<commit_message>
added calculations for column mean and the median
</commit_message>
<xml_diff>
--- a/data/Sales Records processed.xlsx
+++ b/data/Sales Records processed.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N1002"/>
+  <dimension ref="A1:N1004"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -54542,6 +54542,98 @@
         <v>388452710.08</v>
       </c>
     </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>Median</t>
+        </is>
+      </c>
+      <c r="B1003" t="n">
+        <v/>
+      </c>
+      <c r="C1003" t="n">
+        <v/>
+      </c>
+      <c r="D1003" t="n">
+        <v/>
+      </c>
+      <c r="E1003" t="n">
+        <v/>
+      </c>
+      <c r="F1003" t="n">
+        <v/>
+      </c>
+      <c r="G1003" t="n">
+        <v/>
+      </c>
+      <c r="H1003" t="n">
+        <v/>
+      </c>
+      <c r="I1003" t="n">
+        <v>4819</v>
+      </c>
+      <c r="J1003" t="n">
+        <v>154.06</v>
+      </c>
+      <c r="K1003" t="n">
+        <v>97.44</v>
+      </c>
+      <c r="L1003" t="n">
+        <v>766026.8</v>
+      </c>
+      <c r="M1003" t="n">
+        <v>452278.82</v>
+      </c>
+      <c r="N1003" t="n">
+        <v>273211.56</v>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>Mean</t>
+        </is>
+      </c>
+      <c r="B1004" t="n">
+        <v/>
+      </c>
+      <c r="C1004" t="n">
+        <v/>
+      </c>
+      <c r="D1004" t="n">
+        <v/>
+      </c>
+      <c r="E1004" t="n">
+        <v/>
+      </c>
+      <c r="F1004" t="n">
+        <v/>
+      </c>
+      <c r="G1004" t="n">
+        <v/>
+      </c>
+      <c r="H1004" t="n">
+        <v/>
+      </c>
+      <c r="I1004" t="n">
+        <v>9838.995009980041</v>
+      </c>
+      <c r="J1004" t="n">
+        <v>267.7777722277724</v>
+      </c>
+      <c r="K1004" t="n">
+        <v>188.652867132867</v>
+      </c>
+      <c r="L1004" t="n">
+        <v>2596379.357844312</v>
+      </c>
+      <c r="M1004" t="n">
+        <v>1820711.525369262</v>
+      </c>
+      <c r="N1004" t="n">
+        <v>775627.3769660678</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added more styling at the bottom of the sheet
</commit_message>
<xml_diff>
--- a/data/Sales Records processed.xlsx
+++ b/data/Sales Records processed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmad\Desktop\Ahmad\python\excel\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C933E3D6-0C3D-47CD-9C3B-FBFA3EF5A49F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6EA7E10-43C2-4672-8778-E6691C9D2515}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4650" yWindow="1545" windowWidth="22815" windowHeight="12780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -197,7 +197,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,6 +211,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -220,7 +226,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -237,14 +243,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,8 +580,8 @@
   <dimension ref="A1:N1004"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <pane ySplit="1" topLeftCell="A978" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B981" sqref="B981"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,10 +593,10 @@
     <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -44614,65 +44644,88 @@
       </c>
     </row>
     <row r="1002" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1002" t="s">
+      <c r="A1002" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="I1002">
+      <c r="B1002" s="3"/>
+      <c r="C1002" s="3"/>
+      <c r="D1002" s="3"/>
+      <c r="E1002" s="3"/>
+      <c r="F1002" s="3"/>
+      <c r="G1002" s="3"/>
+      <c r="H1002" s="3"/>
+      <c r="I1002" s="3">
         <v>4926927</v>
       </c>
-      <c r="L1002">
+      <c r="J1002" s="3"/>
+      <c r="K1002" s="3"/>
+      <c r="L1002" s="3">
         <v>1300403044.8800001</v>
       </c>
-      <c r="M1002">
+      <c r="M1002" s="3">
         <v>911950334.80000007</v>
       </c>
-      <c r="N1002">
+      <c r="N1002" s="3">
         <v>388452710.07999998</v>
       </c>
     </row>
     <row r="1003" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1003" t="s">
+      <c r="A1003" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I1003">
+      <c r="B1003" s="3"/>
+      <c r="C1003" s="3"/>
+      <c r="D1003" s="3"/>
+      <c r="E1003" s="3"/>
+      <c r="F1003" s="3"/>
+      <c r="G1003" s="3"/>
+      <c r="H1003" s="3"/>
+      <c r="I1003" s="3">
         <v>4819</v>
       </c>
-      <c r="J1003">
+      <c r="J1003" s="3">
         <v>154.06</v>
       </c>
-      <c r="K1003">
+      <c r="K1003" s="3">
         <v>97.44</v>
       </c>
-      <c r="L1003">
+      <c r="L1003" s="3">
         <v>766026.8</v>
       </c>
-      <c r="M1003">
+      <c r="M1003" s="3">
         <v>452278.82</v>
       </c>
-      <c r="N1003">
+      <c r="N1003" s="3">
         <v>273211.56</v>
       </c>
     </row>
     <row r="1004" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1004" t="s">
+      <c r="A1004" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="I1004">
+      <c r="B1004" s="4"/>
+      <c r="C1004" s="4"/>
+      <c r="D1004" s="4"/>
+      <c r="E1004" s="4"/>
+      <c r="F1004" s="4"/>
+      <c r="G1004" s="4"/>
+      <c r="H1004" s="4"/>
+      <c r="I1004" s="4">
         <v>9838.9950099800408</v>
       </c>
-      <c r="J1004">
+      <c r="J1004" s="4">
         <v>267.7777722277724</v>
       </c>
-      <c r="K1004">
+      <c r="K1004" s="4">
         <v>188.65286713286699</v>
       </c>
-      <c r="L1004">
+      <c r="L1004" s="4">
         <v>2596379.3578443122</v>
       </c>
-      <c r="M1004">
+      <c r="M1004" s="4">
         <v>1820711.5253692621</v>
       </c>
-      <c r="N1004">
+      <c r="N1004" s="4">
         <v>775627.37696606782</v>
       </c>
     </row>

</xml_diff>

<commit_message>
edited some scenarios and added numeric formating
</commit_message>
<xml_diff>
--- a/data/Sales Records processed.xlsx
+++ b/data/Sales Records processed.xlsx
@@ -17,8 +17,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="$#,###"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -88,13 +89,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -62727,12 +62729,12 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Scenario</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Value</t>
         </is>
@@ -62741,51 +62743,51 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>number of orders with total revenue over $2m</t>
+          <t>number of orders for household items</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>209</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>sum of revenue for orders with total revenue over $2m</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>2071243530.28</v>
+          <t>sum of revenue for household items</t>
+        </is>
+      </c>
+      <c r="B3" s="6" t="n">
+        <v>254481893.89</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>average of revenue for orders with total revenue over $2m</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>9910256</v>
+          <t>average revenue for household items</t>
+        </is>
+      </c>
+      <c r="B4" s="6" t="n">
+        <v>3029546</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>average of revenue for orders with total revenue over $500k, medium priority</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>1998135</v>
+          <t>average revenue for household items ordered with medium priority</t>
+        </is>
+      </c>
+      <c r="B5" s="6" t="n">
+        <v>2687197</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>average of revenue for household item orders with total revenue over $100k, high priority</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>2834292</v>
+          <t>average for high revenue orders (&gt; $1m) for household items ordered with high priority</t>
+        </is>
+      </c>
+      <c r="B6" s="6" t="n">
+        <v>3323032</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added more sumif and averageif scenarios
</commit_message>
<xml_diff>
--- a/data/Sales Records processed.xlsx
+++ b/data/Sales Records processed.xlsx
@@ -62720,7 +62720,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -62773,20 +62773,30 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>average revenue for household items ordered with medium priority</t>
+          <t>sum revenue for household items ordered with medium priority</t>
         </is>
       </c>
       <c r="B5" s="6" t="n">
-        <v>2687197</v>
+        <v>42995155.26</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>average revenue for household items ordered with medium priority</t>
+        </is>
+      </c>
+      <c r="B6" s="6" t="n">
+        <v>2687197</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>average for high revenue orders (&gt; $1m) for household items ordered with high priority</t>
         </is>
       </c>
-      <c r="B6" s="6" t="n">
+      <c r="B7" s="6" t="n">
         <v>3323032</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added summary table calculating average profit per country
</commit_message>
<xml_diff>
--- a/data/Sales Records processed.xlsx
+++ b/data/Sales Records processed.xlsx
@@ -18,9 +18,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="$#,###"/>
+    <numFmt numFmtId="166" formatCode="$#,###.##"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -90,7 +91,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -98,6 +99,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -62812,7 +62814,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -62821,15 +62823,205 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Scenario</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Value</t>
-        </is>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Average Profit</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Antigua and Barbuda </t>
+        </is>
+      </c>
+      <c r="B2" s="7" t="n">
+        <v>1494586.52</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Barbados</t>
+        </is>
+      </c>
+      <c r="B3" s="7" t="n">
+        <v>1322524.768</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Belize</t>
+        </is>
+      </c>
+      <c r="B4" s="7" t="n">
+        <v>1137689.366666667</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Costa Rica</t>
+        </is>
+      </c>
+      <c r="B5" s="7" t="n">
+        <v>982148.1625</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Cuba</t>
+        </is>
+      </c>
+      <c r="B6" s="7" t="n">
+        <v>877927.5866666668</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Dominica</t>
+        </is>
+      </c>
+      <c r="B7" s="7" t="n">
+        <v>926379.3600000001</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Dominican Republic</t>
+        </is>
+      </c>
+      <c r="B8" s="7" t="n">
+        <v>913165.24</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>El Salvador</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="n">
+        <v>694436.78</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Grenada</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="n">
+        <v>1110751.108</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Guatemala</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="n">
+        <v>949764.8750000001</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Haiti</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="n">
+        <v>828360.1475</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Honduras</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="n">
+        <v>1391307.74</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Jamaica</t>
+        </is>
+      </c>
+      <c r="B14" s="7" t="n">
+        <v>1354795.04</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Nicaragua</t>
+        </is>
+      </c>
+      <c r="B15" s="7" t="n">
+        <v>706491.7666666666</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Panama</t>
+        </is>
+      </c>
+      <c r="B16" s="7" t="n">
+        <v>1015922.41</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Saint Kitts and Nevis </t>
+        </is>
+      </c>
+      <c r="B17" s="7" t="n">
+        <v>556963.5666666667</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Saint Lucia</t>
+        </is>
+      </c>
+      <c r="B18" s="7" t="n">
+        <v>971498.625</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Saint Vincent and the Grenadines</t>
+        </is>
+      </c>
+      <c r="B19" s="7" t="n">
+        <v>1636812.18</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>The Bahamas</t>
+        </is>
+      </c>
+      <c r="B20" s="7" t="n">
+        <v>526478.36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
multiple summary tables in the same worksheet
</commit_message>
<xml_diff>
--- a/data/Sales Records processed.xlsx
+++ b/data/Sales Records processed.xlsx
@@ -10,6 +10,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="americas" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="americas2" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="cosmetics" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="summary" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -63027,4 +63028,657 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B64"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Fruits Average Profit</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Antigua and Barbuda </t>
+        </is>
+      </c>
+      <c r="B2" s="7" t="n">
+        <v>11075.95833333333</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Barbados</t>
+        </is>
+      </c>
+      <c r="B3" s="7" t="n">
+        <v>19446.772</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Belize</t>
+        </is>
+      </c>
+      <c r="B4" s="7" t="n">
+        <v>14858.855</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Costa Rica</t>
+        </is>
+      </c>
+      <c r="B5" s="7" t="n">
+        <v>16768.78</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Cuba</t>
+        </is>
+      </c>
+      <c r="B6" s="7" t="n">
+        <v>16987.05714285714</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Dominica</t>
+        </is>
+      </c>
+      <c r="B7" s="7" t="n">
+        <v>9404.422500000001</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Dominican Republic</t>
+        </is>
+      </c>
+      <c r="B8" s="7" t="n">
+        <v>14326.64666666667</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>El Salvador</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="n">
+        <v>11365.078</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Grenada</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="n">
+        <v>4953.755</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Guatemala</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="n">
+        <v>14475.665</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Haiti</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="n">
+        <v>13817.735</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Honduras</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="n">
+        <v>8104.829999999999</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Jamaica</t>
+        </is>
+      </c>
+      <c r="B14" s="7" t="n">
+        <v>12800.31333333333</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Nicaragua</t>
+        </is>
+      </c>
+      <c r="B15" s="7" t="n">
+        <v>10933.5675</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Panama</t>
+        </is>
+      </c>
+      <c r="B16" s="7" t="n">
+        <v>8833.453333333333</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Saint Kitts and Nevis </t>
+        </is>
+      </c>
+      <c r="B17" s="7" t="n">
+        <v>7222.288</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Saint Lucia</t>
+        </is>
+      </c>
+      <c r="B18" s="7" t="n">
+        <v>15414.9625</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Saint Vincent and the Grenadines</t>
+        </is>
+      </c>
+      <c r="B19" s="7" t="n">
+        <v>19132.99</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>The Bahamas</t>
+        </is>
+      </c>
+      <c r="B20" s="7" t="n">
+        <v>8022.889999999999</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Trinidad and Tobago</t>
+        </is>
+      </c>
+      <c r="B21" s="7" t="n">
+        <v>13059.79</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr"/>
+      <c r="B22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="B23" s="1" t="inlineStr">
+        <is>
+          <t>Vegetables Average Profit</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Antigua and Barbuda </t>
+        </is>
+      </c>
+      <c r="B24" s="7" t="n">
+        <v>140558.945</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Barbados</t>
+        </is>
+      </c>
+      <c r="B25" s="7" t="n">
+        <v>166647.4175</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Belize</t>
+        </is>
+      </c>
+      <c r="B26" s="7" t="n">
+        <v>347494.5757142857</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Costa Rica</t>
+        </is>
+      </c>
+      <c r="B27" s="7" t="n">
+        <v>428625.6442857143</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Cuba</t>
+        </is>
+      </c>
+      <c r="B28" s="7" t="n">
+        <v>571137.11</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Dominica</t>
+        </is>
+      </c>
+      <c r="B29" s="7" t="n">
+        <v>309673.6933333333</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Dominican Republic</t>
+        </is>
+      </c>
+      <c r="B30" s="7" t="n">
+        <v>237255.166</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>El Salvador</t>
+        </is>
+      </c>
+      <c r="B31" s="7" t="n">
+        <v>308937.1766666667</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Grenada</t>
+        </is>
+      </c>
+      <c r="B32" s="7" t="n">
+        <v>408787.7933333333</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Guatemala</t>
+        </is>
+      </c>
+      <c r="B33" s="7" t="n">
+        <v>232665.615</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Haiti</t>
+        </is>
+      </c>
+      <c r="B34" s="7" t="n">
+        <v>448336.634</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Honduras</t>
+        </is>
+      </c>
+      <c r="B35" s="7" t="n">
+        <v>427326.97</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Jamaica</t>
+        </is>
+      </c>
+      <c r="B36" s="7" t="n">
+        <v>478588.53</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Nicaragua</t>
+        </is>
+      </c>
+      <c r="B37" s="7" t="n">
+        <v>310902.624</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Panama</t>
+        </is>
+      </c>
+      <c r="B38" s="7" t="n">
+        <v>434239.7050000001</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Saint Kitts and Nevis </t>
+        </is>
+      </c>
+      <c r="B39" s="7" t="n">
+        <v>317846.924</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Saint Lucia</t>
+        </is>
+      </c>
+      <c r="B40" s="7" t="n">
+        <v>377559.4866666666</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Saint Vincent and the Grenadines</t>
+        </is>
+      </c>
+      <c r="B41" s="7" t="n">
+        <v>267308.2025</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>The Bahamas</t>
+        </is>
+      </c>
+      <c r="B42" s="7" t="n">
+        <v>253372.255</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Trinidad and Tobago</t>
+        </is>
+      </c>
+      <c r="B43" s="7" t="n">
+        <v>274599.7175</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr"/>
+      <c r="B44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="B45" s="1" t="inlineStr">
+        <is>
+          <t>Meat Average Profit</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Antigua and Barbuda </t>
+        </is>
+      </c>
+      <c r="B46" s="7" t="n">
+        <v>130358.8</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Barbados</t>
+        </is>
+      </c>
+      <c r="B47" s="7" t="n">
+        <v>273621.92</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Belize</t>
+        </is>
+      </c>
+      <c r="B48" s="7" t="n">
+        <v>280070.2666666667</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Costa Rica</t>
+        </is>
+      </c>
+      <c r="B49" s="7" t="n">
+        <v>331331</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Cuba</t>
+        </is>
+      </c>
+      <c r="B50" s="7" t="n">
+        <v>233070.9333333333</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Dominica</t>
+        </is>
+      </c>
+      <c r="B51" s="7" t="n">
+        <v>290278.56</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Dominican Republic</t>
+        </is>
+      </c>
+      <c r="B52" s="7" t="n">
+        <v>303865.4666666667</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>El Salvador</t>
+        </is>
+      </c>
+      <c r="B53" s="7" t="n">
+        <v>389627.3333333333</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Grenada</t>
+        </is>
+      </c>
+      <c r="B54" s="7" t="n">
+        <v>471030.5599999999</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Guatemala</t>
+        </is>
+      </c>
+      <c r="B55" s="7" t="n">
+        <v>321476.7111111111</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Haiti</t>
+        </is>
+      </c>
+      <c r="B56" s="7" t="n">
+        <v>205557.7333333333</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Honduras</t>
+        </is>
+      </c>
+      <c r="B57" s="7" t="n">
+        <v>173258.8</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Jamaica</t>
+        </is>
+      </c>
+      <c r="B58" s="7" t="n">
+        <v>262147.6</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Nicaragua</t>
+        </is>
+      </c>
+      <c r="B59" s="7" t="n">
+        <v>300299.9999999999</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Panama</t>
+        </is>
+      </c>
+      <c r="B60" s="7" t="n">
+        <v>343900.7</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Saint Lucia</t>
+        </is>
+      </c>
+      <c r="B61" s="7" t="n">
+        <v>320262.8</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Saint Vincent and the Grenadines</t>
+        </is>
+      </c>
+      <c r="B62" s="7" t="n">
+        <v>312712.4</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>The Bahamas</t>
+        </is>
+      </c>
+      <c r="B63" s="7" t="n">
+        <v>184327</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Trinidad and Tobago</t>
+        </is>
+      </c>
+      <c r="B64" s="7" t="n">
+        <v>293756.3199999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding an alternate summary table method
</commit_message>
<xml_diff>
--- a/data/Sales Records processed.xlsx
+++ b/data/Sales Records processed.xlsx
@@ -11,6 +11,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="americas2" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="cosmetics" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="summary" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="summary2" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -63681,4 +63682,22 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added a new sheet for alternative summary tables
</commit_message>
<xml_diff>
--- a/data/Sales Records processed.xlsx
+++ b/data/Sales Records processed.xlsx
@@ -63690,14 +63690,357 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Fruit Avg Profit</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Vegetables Avg Profit</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Meat Avg Profit</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Antigua and Barbuda </t>
+        </is>
+      </c>
+      <c r="B2" s="7" t="n">
+        <v>11075.95833333333</v>
+      </c>
+      <c r="C2" s="7" t="n">
+        <v>140558.945</v>
+      </c>
+      <c r="D2" s="7" t="n">
+        <v>130358.8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Barbados</t>
+        </is>
+      </c>
+      <c r="B3" s="7" t="n">
+        <v>19446.772</v>
+      </c>
+      <c r="C3" s="7" t="n">
+        <v>166647.4175</v>
+      </c>
+      <c r="D3" s="7" t="n">
+        <v>273621.92</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Belize</t>
+        </is>
+      </c>
+      <c r="B4" s="7" t="n">
+        <v>14858.855</v>
+      </c>
+      <c r="C4" s="7" t="n">
+        <v>347494.5757142857</v>
+      </c>
+      <c r="D4" s="7" t="n">
+        <v>280070.2666666667</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Costa Rica</t>
+        </is>
+      </c>
+      <c r="B5" s="7" t="n">
+        <v>16768.78</v>
+      </c>
+      <c r="C5" s="7" t="n">
+        <v>428625.6442857143</v>
+      </c>
+      <c r="D5" s="7" t="n">
+        <v>331331</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Cuba</t>
+        </is>
+      </c>
+      <c r="B6" s="7" t="n">
+        <v>16987.05714285714</v>
+      </c>
+      <c r="C6" s="7" t="n">
+        <v>571137.11</v>
+      </c>
+      <c r="D6" s="7" t="n">
+        <v>233070.9333333333</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Dominica</t>
+        </is>
+      </c>
+      <c r="B7" s="7" t="n">
+        <v>9404.422500000001</v>
+      </c>
+      <c r="C7" s="7" t="n">
+        <v>309673.6933333333</v>
+      </c>
+      <c r="D7" s="7" t="n">
+        <v>290278.56</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Dominican Republic</t>
+        </is>
+      </c>
+      <c r="B8" s="7" t="n">
+        <v>14326.64666666667</v>
+      </c>
+      <c r="C8" s="7" t="n">
+        <v>237255.166</v>
+      </c>
+      <c r="D8" s="7" t="n">
+        <v>303865.4666666667</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>El Salvador</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="n">
+        <v>11365.078</v>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>308937.1766666667</v>
+      </c>
+      <c r="D9" s="7" t="n">
+        <v>389627.3333333333</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Grenada</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="n">
+        <v>4953.755</v>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>408787.7933333333</v>
+      </c>
+      <c r="D10" s="7" t="n">
+        <v>471030.5599999999</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Guatemala</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="n">
+        <v>14475.665</v>
+      </c>
+      <c r="C11" s="7" t="n">
+        <v>232665.615</v>
+      </c>
+      <c r="D11" s="7" t="n">
+        <v>321476.7111111111</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Haiti</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="n">
+        <v>13817.735</v>
+      </c>
+      <c r="C12" s="7" t="n">
+        <v>448336.634</v>
+      </c>
+      <c r="D12" s="7" t="n">
+        <v>205557.7333333333</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Honduras</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="n">
+        <v>8104.829999999999</v>
+      </c>
+      <c r="C13" s="7" t="n">
+        <v>427326.97</v>
+      </c>
+      <c r="D13" s="7" t="n">
+        <v>173258.8</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Jamaica</t>
+        </is>
+      </c>
+      <c r="B14" s="7" t="n">
+        <v>12800.31333333333</v>
+      </c>
+      <c r="C14" s="7" t="n">
+        <v>478588.53</v>
+      </c>
+      <c r="D14" s="7" t="n">
+        <v>262147.6</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Nicaragua</t>
+        </is>
+      </c>
+      <c r="B15" s="7" t="n">
+        <v>10933.5675</v>
+      </c>
+      <c r="C15" s="7" t="n">
+        <v>310902.624</v>
+      </c>
+      <c r="D15" s="7" t="n">
+        <v>300299.9999999999</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Panama</t>
+        </is>
+      </c>
+      <c r="B16" s="7" t="n">
+        <v>8833.453333333333</v>
+      </c>
+      <c r="C16" s="7" t="n">
+        <v>434239.7050000001</v>
+      </c>
+      <c r="D16" s="7" t="n">
+        <v>343900.7</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Saint Kitts and Nevis </t>
+        </is>
+      </c>
+      <c r="B17" s="7" t="n">
+        <v>7222.288</v>
+      </c>
+      <c r="C17" s="7" t="n">
+        <v>317846.924</v>
+      </c>
+      <c r="D17" s="7" t="n">
+        <v>0.0001</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Saint Lucia</t>
+        </is>
+      </c>
+      <c r="B18" s="7" t="n">
+        <v>15414.9625</v>
+      </c>
+      <c r="C18" s="7" t="n">
+        <v>377559.4866666666</v>
+      </c>
+      <c r="D18" s="7" t="n">
+        <v>320262.8</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Saint Vincent and the Grenadines</t>
+        </is>
+      </c>
+      <c r="B19" s="7" t="n">
+        <v>19132.99</v>
+      </c>
+      <c r="C19" s="7" t="n">
+        <v>267308.2025</v>
+      </c>
+      <c r="D19" s="7" t="n">
+        <v>312712.4</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>The Bahamas</t>
+        </is>
+      </c>
+      <c r="B20" s="7" t="n">
+        <v>8022.889999999999</v>
+      </c>
+      <c r="C20" s="7" t="n">
+        <v>253372.255</v>
+      </c>
+      <c r="D20" s="7" t="n">
+        <v>184327</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Trinidad and Tobago</t>
+        </is>
+      </c>
+      <c r="B21" s="7" t="n">
+        <v>13059.79</v>
+      </c>
+      <c r="C21" s="7" t="n">
+        <v>274599.7175</v>
+      </c>
+      <c r="D21" s="7" t="n">
+        <v>293756.3199999999</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
started coding pivot table creation
</commit_message>
<xml_diff>
--- a/data/Sales Records processed.xlsx
+++ b/data/Sales Records processed.xlsx
@@ -63699,22 +63699,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Country</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Fruit Avg Profit</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Vegetables Avg Profit</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Meat Avg Profit</t>
         </is>

</xml_diff>

<commit_message>
edited column names in the pivot table and saved in excel file
</commit_message>
<xml_diff>
--- a/data/Sales Records processed.xlsx
+++ b/data/Sales Records processed.xlsx
@@ -12,6 +12,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="cosmetics" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="summary" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="summary2" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pivot" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -64043,4 +64044,430 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_C</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_H</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_L</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_M</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Antigua and Barbuda </t>
+        </is>
+      </c>
+      <c r="B2" s="7" t="n">
+        <v>20844485.52</v>
+      </c>
+      <c r="C2" s="7" t="n">
+        <v>7562695.25</v>
+      </c>
+      <c r="D2" s="7" t="n">
+        <v>7591994.429999999</v>
+      </c>
+      <c r="E2" s="7" t="n">
+        <v>22845079.64</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Barbados</t>
+        </is>
+      </c>
+      <c r="B3" s="7" t="n">
+        <v>31150537.48</v>
+      </c>
+      <c r="C3" s="7" t="n">
+        <v>7970994.910000001</v>
+      </c>
+      <c r="D3" s="7" t="n">
+        <v>5236966.48</v>
+      </c>
+      <c r="E3" s="7" t="n">
+        <v>14006520.26</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Belize</t>
+        </is>
+      </c>
+      <c r="B4" s="7" t="n">
+        <v>23618654.58</v>
+      </c>
+      <c r="C4" s="7" t="n">
+        <v>29686017.80999999</v>
+      </c>
+      <c r="D4" s="7" t="n">
+        <v>18419455.99</v>
+      </c>
+      <c r="E4" s="7" t="n">
+        <v>15776467.97</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Costa Rica</t>
+        </is>
+      </c>
+      <c r="B5" s="7" t="n">
+        <v>14426137.55</v>
+      </c>
+      <c r="C5" s="7" t="n">
+        <v>10906584.35</v>
+      </c>
+      <c r="D5" s="7" t="n">
+        <v>10228204.13</v>
+      </c>
+      <c r="E5" s="7" t="n">
+        <v>27916477.07</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Cuba</t>
+        </is>
+      </c>
+      <c r="B6" s="7" t="n">
+        <v>28383625.54</v>
+      </c>
+      <c r="C6" s="7" t="n">
+        <v>7347594.050000001</v>
+      </c>
+      <c r="D6" s="7" t="n">
+        <v>21360945.4</v>
+      </c>
+      <c r="E6" s="7" t="n">
+        <v>18879397.04</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Dominica</t>
+        </is>
+      </c>
+      <c r="B7" s="7" t="n">
+        <v>16812457.3</v>
+      </c>
+      <c r="C7" s="7" t="n">
+        <v>24088504.85</v>
+      </c>
+      <c r="D7" s="7" t="n">
+        <v>22509355.03</v>
+      </c>
+      <c r="E7" s="7" t="n">
+        <v>12265892.81</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Dominican Republic</t>
+        </is>
+      </c>
+      <c r="B8" s="7" t="n">
+        <v>14995299.91</v>
+      </c>
+      <c r="C8" s="7" t="n">
+        <v>11074518.98</v>
+      </c>
+      <c r="D8" s="7" t="n">
+        <v>19854891</v>
+      </c>
+      <c r="E8" s="7" t="n">
+        <v>8476200.93</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>El Salvador</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="n">
+        <v>38434581.36</v>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>27031797.58</v>
+      </c>
+      <c r="D9" s="7" t="n">
+        <v>17026190.84</v>
+      </c>
+      <c r="E9" s="7" t="n">
+        <v>6779478.54</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Grenada</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="n">
+        <v>3346710.4</v>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>27220703.25</v>
+      </c>
+      <c r="D10" s="7" t="n">
+        <v>21895391</v>
+      </c>
+      <c r="E10" s="7" t="n">
+        <v>12353932.49</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Guatemala</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="n">
+        <v>16387275.43</v>
+      </c>
+      <c r="C11" s="7" t="n">
+        <v>19050366.15</v>
+      </c>
+      <c r="D11" s="7" t="n">
+        <v>10633697.7</v>
+      </c>
+      <c r="E11" s="7" t="n">
+        <v>25226077.99</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Haiti</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="n">
+        <v>15417306.97</v>
+      </c>
+      <c r="C12" s="7" t="n">
+        <v>22873523.91</v>
+      </c>
+      <c r="D12" s="7" t="n">
+        <v>17741739.31</v>
+      </c>
+      <c r="E12" s="7" t="n">
+        <v>22056090.19</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Honduras</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="n">
+        <v>3718358.9</v>
+      </c>
+      <c r="C13" s="7" t="n">
+        <v>16853038.42</v>
+      </c>
+      <c r="D13" s="7" t="n">
+        <v>17299349.8</v>
+      </c>
+      <c r="E13" s="7" t="n">
+        <v>5282550.380000001</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Jamaica</t>
+        </is>
+      </c>
+      <c r="B14" s="7" t="n">
+        <v>17235060.29</v>
+      </c>
+      <c r="C14" s="7" t="n">
+        <v>14439360.88</v>
+      </c>
+      <c r="D14" s="7" t="n">
+        <v>18068028.48</v>
+      </c>
+      <c r="E14" s="7" t="n">
+        <v>13593606.87</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Nicaragua</t>
+        </is>
+      </c>
+      <c r="B15" s="7" t="n">
+        <v>18719501.43</v>
+      </c>
+      <c r="C15" s="7" t="n">
+        <v>15660293.96</v>
+      </c>
+      <c r="D15" s="7" t="n">
+        <v>15815870.61</v>
+      </c>
+      <c r="E15" s="7" t="n">
+        <v>16635780.44</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Panama</t>
+        </is>
+      </c>
+      <c r="B16" s="7" t="n">
+        <v>16763511.6</v>
+      </c>
+      <c r="C16" s="7" t="n">
+        <v>15420040.16</v>
+      </c>
+      <c r="D16" s="7" t="n">
+        <v>22289199.21</v>
+      </c>
+      <c r="E16" s="7" t="n">
+        <v>14905937.27</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Saint Kitts and Nevis </t>
+        </is>
+      </c>
+      <c r="B17" s="7" t="n">
+        <v>5075519.199999999</v>
+      </c>
+      <c r="C17" s="7" t="n">
+        <v>19630258.58</v>
+      </c>
+      <c r="D17" s="7" t="n">
+        <v>16493934.3</v>
+      </c>
+      <c r="E17" s="7" t="n">
+        <v>12834909.92</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Saint Lucia</t>
+        </is>
+      </c>
+      <c r="B18" s="7" t="n">
+        <v>16895401.71</v>
+      </c>
+      <c r="C18" s="7" t="n">
+        <v>19765416.97</v>
+      </c>
+      <c r="D18" s="7" t="n">
+        <v>4047144.81</v>
+      </c>
+      <c r="E18" s="7" t="n">
+        <v>16610776.02</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Saint Vincent and the Grenadines</t>
+        </is>
+      </c>
+      <c r="B19" s="7" t="n">
+        <v>20125659.52</v>
+      </c>
+      <c r="C19" s="7" t="n">
+        <v>6937982.4</v>
+      </c>
+      <c r="D19" s="7" t="n">
+        <v>18674500.42</v>
+      </c>
+      <c r="E19" s="7" t="n">
+        <v>20424202.96</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>The Bahamas</t>
+        </is>
+      </c>
+      <c r="B20" s="7" t="n">
+        <v>13069819.29</v>
+      </c>
+      <c r="C20" s="7" t="n">
+        <v>20341693.41</v>
+      </c>
+      <c r="D20" s="7" t="n">
+        <v>10001243.94</v>
+      </c>
+      <c r="E20" s="7" t="n">
+        <v>17570027.04</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Trinidad and Tobago</t>
+        </is>
+      </c>
+      <c r="B21" s="7" t="n">
+        <v>8991682.289999999</v>
+      </c>
+      <c r="C21" s="7" t="n">
+        <v>7274585.720000003</v>
+      </c>
+      <c r="D21" s="7" t="n">
+        <v>12156780.74</v>
+      </c>
+      <c r="E21" s="7" t="n">
+        <v>13071197.57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed number formatting in the pivot table
</commit_message>
<xml_diff>
--- a/data/Sales Records processed.xlsx
+++ b/data/Sales Records processed.xlsx
@@ -64093,16 +64093,16 @@
           <t xml:space="preserve">Antigua and Barbuda </t>
         </is>
       </c>
-      <c r="B2" s="7" t="n">
+      <c r="B2" s="6" t="n">
         <v>20844485.52</v>
       </c>
-      <c r="C2" s="7" t="n">
+      <c r="C2" s="6" t="n">
         <v>7562695.25</v>
       </c>
-      <c r="D2" s="7" t="n">
+      <c r="D2" s="6" t="n">
         <v>7591994.429999999</v>
       </c>
-      <c r="E2" s="7" t="n">
+      <c r="E2" s="6" t="n">
         <v>22845079.64</v>
       </c>
     </row>
@@ -64112,16 +64112,16 @@
           <t>Barbados</t>
         </is>
       </c>
-      <c r="B3" s="7" t="n">
+      <c r="B3" s="6" t="n">
         <v>31150537.48</v>
       </c>
-      <c r="C3" s="7" t="n">
+      <c r="C3" s="6" t="n">
         <v>7970994.910000001</v>
       </c>
-      <c r="D3" s="7" t="n">
+      <c r="D3" s="6" t="n">
         <v>5236966.48</v>
       </c>
-      <c r="E3" s="7" t="n">
+      <c r="E3" s="6" t="n">
         <v>14006520.26</v>
       </c>
     </row>
@@ -64131,16 +64131,16 @@
           <t>Belize</t>
         </is>
       </c>
-      <c r="B4" s="7" t="n">
+      <c r="B4" s="6" t="n">
         <v>23618654.58</v>
       </c>
-      <c r="C4" s="7" t="n">
+      <c r="C4" s="6" t="n">
         <v>29686017.80999999</v>
       </c>
-      <c r="D4" s="7" t="n">
+      <c r="D4" s="6" t="n">
         <v>18419455.99</v>
       </c>
-      <c r="E4" s="7" t="n">
+      <c r="E4" s="6" t="n">
         <v>15776467.97</v>
       </c>
     </row>
@@ -64150,16 +64150,16 @@
           <t>Costa Rica</t>
         </is>
       </c>
-      <c r="B5" s="7" t="n">
+      <c r="B5" s="6" t="n">
         <v>14426137.55</v>
       </c>
-      <c r="C5" s="7" t="n">
+      <c r="C5" s="6" t="n">
         <v>10906584.35</v>
       </c>
-      <c r="D5" s="7" t="n">
+      <c r="D5" s="6" t="n">
         <v>10228204.13</v>
       </c>
-      <c r="E5" s="7" t="n">
+      <c r="E5" s="6" t="n">
         <v>27916477.07</v>
       </c>
     </row>
@@ -64169,16 +64169,16 @@
           <t>Cuba</t>
         </is>
       </c>
-      <c r="B6" s="7" t="n">
+      <c r="B6" s="6" t="n">
         <v>28383625.54</v>
       </c>
-      <c r="C6" s="7" t="n">
+      <c r="C6" s="6" t="n">
         <v>7347594.050000001</v>
       </c>
-      <c r="D6" s="7" t="n">
+      <c r="D6" s="6" t="n">
         <v>21360945.4</v>
       </c>
-      <c r="E6" s="7" t="n">
+      <c r="E6" s="6" t="n">
         <v>18879397.04</v>
       </c>
     </row>
@@ -64188,16 +64188,16 @@
           <t>Dominica</t>
         </is>
       </c>
-      <c r="B7" s="7" t="n">
+      <c r="B7" s="6" t="n">
         <v>16812457.3</v>
       </c>
-      <c r="C7" s="7" t="n">
+      <c r="C7" s="6" t="n">
         <v>24088504.85</v>
       </c>
-      <c r="D7" s="7" t="n">
+      <c r="D7" s="6" t="n">
         <v>22509355.03</v>
       </c>
-      <c r="E7" s="7" t="n">
+      <c r="E7" s="6" t="n">
         <v>12265892.81</v>
       </c>
     </row>
@@ -64207,16 +64207,16 @@
           <t>Dominican Republic</t>
         </is>
       </c>
-      <c r="B8" s="7" t="n">
+      <c r="B8" s="6" t="n">
         <v>14995299.91</v>
       </c>
-      <c r="C8" s="7" t="n">
+      <c r="C8" s="6" t="n">
         <v>11074518.98</v>
       </c>
-      <c r="D8" s="7" t="n">
+      <c r="D8" s="6" t="n">
         <v>19854891</v>
       </c>
-      <c r="E8" s="7" t="n">
+      <c r="E8" s="6" t="n">
         <v>8476200.93</v>
       </c>
     </row>
@@ -64226,16 +64226,16 @@
           <t>El Salvador</t>
         </is>
       </c>
-      <c r="B9" s="7" t="n">
+      <c r="B9" s="6" t="n">
         <v>38434581.36</v>
       </c>
-      <c r="C9" s="7" t="n">
+      <c r="C9" s="6" t="n">
         <v>27031797.58</v>
       </c>
-      <c r="D9" s="7" t="n">
+      <c r="D9" s="6" t="n">
         <v>17026190.84</v>
       </c>
-      <c r="E9" s="7" t="n">
+      <c r="E9" s="6" t="n">
         <v>6779478.54</v>
       </c>
     </row>
@@ -64245,16 +64245,16 @@
           <t>Grenada</t>
         </is>
       </c>
-      <c r="B10" s="7" t="n">
+      <c r="B10" s="6" t="n">
         <v>3346710.4</v>
       </c>
-      <c r="C10" s="7" t="n">
+      <c r="C10" s="6" t="n">
         <v>27220703.25</v>
       </c>
-      <c r="D10" s="7" t="n">
+      <c r="D10" s="6" t="n">
         <v>21895391</v>
       </c>
-      <c r="E10" s="7" t="n">
+      <c r="E10" s="6" t="n">
         <v>12353932.49</v>
       </c>
     </row>
@@ -64264,16 +64264,16 @@
           <t>Guatemala</t>
         </is>
       </c>
-      <c r="B11" s="7" t="n">
+      <c r="B11" s="6" t="n">
         <v>16387275.43</v>
       </c>
-      <c r="C11" s="7" t="n">
+      <c r="C11" s="6" t="n">
         <v>19050366.15</v>
       </c>
-      <c r="D11" s="7" t="n">
+      <c r="D11" s="6" t="n">
         <v>10633697.7</v>
       </c>
-      <c r="E11" s="7" t="n">
+      <c r="E11" s="6" t="n">
         <v>25226077.99</v>
       </c>
     </row>
@@ -64283,16 +64283,16 @@
           <t>Haiti</t>
         </is>
       </c>
-      <c r="B12" s="7" t="n">
+      <c r="B12" s="6" t="n">
         <v>15417306.97</v>
       </c>
-      <c r="C12" s="7" t="n">
+      <c r="C12" s="6" t="n">
         <v>22873523.91</v>
       </c>
-      <c r="D12" s="7" t="n">
+      <c r="D12" s="6" t="n">
         <v>17741739.31</v>
       </c>
-      <c r="E12" s="7" t="n">
+      <c r="E12" s="6" t="n">
         <v>22056090.19</v>
       </c>
     </row>
@@ -64302,16 +64302,16 @@
           <t>Honduras</t>
         </is>
       </c>
-      <c r="B13" s="7" t="n">
+      <c r="B13" s="6" t="n">
         <v>3718358.9</v>
       </c>
-      <c r="C13" s="7" t="n">
+      <c r="C13" s="6" t="n">
         <v>16853038.42</v>
       </c>
-      <c r="D13" s="7" t="n">
+      <c r="D13" s="6" t="n">
         <v>17299349.8</v>
       </c>
-      <c r="E13" s="7" t="n">
+      <c r="E13" s="6" t="n">
         <v>5282550.380000001</v>
       </c>
     </row>
@@ -64321,16 +64321,16 @@
           <t>Jamaica</t>
         </is>
       </c>
-      <c r="B14" s="7" t="n">
+      <c r="B14" s="6" t="n">
         <v>17235060.29</v>
       </c>
-      <c r="C14" s="7" t="n">
+      <c r="C14" s="6" t="n">
         <v>14439360.88</v>
       </c>
-      <c r="D14" s="7" t="n">
+      <c r="D14" s="6" t="n">
         <v>18068028.48</v>
       </c>
-      <c r="E14" s="7" t="n">
+      <c r="E14" s="6" t="n">
         <v>13593606.87</v>
       </c>
     </row>
@@ -64340,16 +64340,16 @@
           <t>Nicaragua</t>
         </is>
       </c>
-      <c r="B15" s="7" t="n">
+      <c r="B15" s="6" t="n">
         <v>18719501.43</v>
       </c>
-      <c r="C15" s="7" t="n">
+      <c r="C15" s="6" t="n">
         <v>15660293.96</v>
       </c>
-      <c r="D15" s="7" t="n">
+      <c r="D15" s="6" t="n">
         <v>15815870.61</v>
       </c>
-      <c r="E15" s="7" t="n">
+      <c r="E15" s="6" t="n">
         <v>16635780.44</v>
       </c>
     </row>
@@ -64359,16 +64359,16 @@
           <t>Panama</t>
         </is>
       </c>
-      <c r="B16" s="7" t="n">
+      <c r="B16" s="6" t="n">
         <v>16763511.6</v>
       </c>
-      <c r="C16" s="7" t="n">
+      <c r="C16" s="6" t="n">
         <v>15420040.16</v>
       </c>
-      <c r="D16" s="7" t="n">
+      <c r="D16" s="6" t="n">
         <v>22289199.21</v>
       </c>
-      <c r="E16" s="7" t="n">
+      <c r="E16" s="6" t="n">
         <v>14905937.27</v>
       </c>
     </row>
@@ -64378,16 +64378,16 @@
           <t xml:space="preserve">Saint Kitts and Nevis </t>
         </is>
       </c>
-      <c r="B17" s="7" t="n">
+      <c r="B17" s="6" t="n">
         <v>5075519.199999999</v>
       </c>
-      <c r="C17" s="7" t="n">
+      <c r="C17" s="6" t="n">
         <v>19630258.58</v>
       </c>
-      <c r="D17" s="7" t="n">
+      <c r="D17" s="6" t="n">
         <v>16493934.3</v>
       </c>
-      <c r="E17" s="7" t="n">
+      <c r="E17" s="6" t="n">
         <v>12834909.92</v>
       </c>
     </row>
@@ -64397,16 +64397,16 @@
           <t>Saint Lucia</t>
         </is>
       </c>
-      <c r="B18" s="7" t="n">
+      <c r="B18" s="6" t="n">
         <v>16895401.71</v>
       </c>
-      <c r="C18" s="7" t="n">
+      <c r="C18" s="6" t="n">
         <v>19765416.97</v>
       </c>
-      <c r="D18" s="7" t="n">
+      <c r="D18" s="6" t="n">
         <v>4047144.81</v>
       </c>
-      <c r="E18" s="7" t="n">
+      <c r="E18" s="6" t="n">
         <v>16610776.02</v>
       </c>
     </row>
@@ -64416,16 +64416,16 @@
           <t>Saint Vincent and the Grenadines</t>
         </is>
       </c>
-      <c r="B19" s="7" t="n">
+      <c r="B19" s="6" t="n">
         <v>20125659.52</v>
       </c>
-      <c r="C19" s="7" t="n">
+      <c r="C19" s="6" t="n">
         <v>6937982.4</v>
       </c>
-      <c r="D19" s="7" t="n">
+      <c r="D19" s="6" t="n">
         <v>18674500.42</v>
       </c>
-      <c r="E19" s="7" t="n">
+      <c r="E19" s="6" t="n">
         <v>20424202.96</v>
       </c>
     </row>
@@ -64435,16 +64435,16 @@
           <t>The Bahamas</t>
         </is>
       </c>
-      <c r="B20" s="7" t="n">
+      <c r="B20" s="6" t="n">
         <v>13069819.29</v>
       </c>
-      <c r="C20" s="7" t="n">
+      <c r="C20" s="6" t="n">
         <v>20341693.41</v>
       </c>
-      <c r="D20" s="7" t="n">
+      <c r="D20" s="6" t="n">
         <v>10001243.94</v>
       </c>
-      <c r="E20" s="7" t="n">
+      <c r="E20" s="6" t="n">
         <v>17570027.04</v>
       </c>
     </row>
@@ -64454,16 +64454,16 @@
           <t>Trinidad and Tobago</t>
         </is>
       </c>
-      <c r="B21" s="7" t="n">
+      <c r="B21" s="6" t="n">
         <v>8991682.289999999</v>
       </c>
-      <c r="C21" s="7" t="n">
+      <c r="C21" s="6" t="n">
         <v>7274585.720000003</v>
       </c>
-      <c r="D21" s="7" t="n">
+      <c r="D21" s="6" t="n">
         <v>12156780.74</v>
       </c>
-      <c r="E21" s="7" t="n">
+      <c r="E21" s="6" t="n">
         <v>13071197.57</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added a second pivot table with two level columns
</commit_message>
<xml_diff>
--- a/data/Sales Records processed.xlsx
+++ b/data/Sales Records processed.xlsx
@@ -13,6 +13,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="summary" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="summary2" sheetId="5" state="visible" r:id="rId5"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pivot" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pivot_2" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -64470,4 +64471,3290 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AW21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Baby Food_C</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Baby Food_H</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Baby Food_L</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Baby Food_M</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Beverages_C</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Beverages_H</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Beverages_L</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Beverages_M</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Cereal_C</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Cereal_H</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Cereal_L</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Cereal_M</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Clothes_C</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Clothes_H</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Clothes_L</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Clothes_M</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Cosmetics_C</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Cosmetics_H</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Cosmetics_L</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Cosmetics_M</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Fruits_C</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Fruits_H</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Fruits_L</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Fruits_M</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Household_C</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Household_H</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Household_L</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Household_M</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Meat_C</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Meat_H</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Meat_L</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Meat_M</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Office Supplies_C</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Office Supplies_H</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Office Supplies_L</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Office Supplies_M</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Personal Care_C</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Personal Care_H</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Personal Care_L</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Personal Care_M</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Snacks_C</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Snacks_H</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Snacks_L</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Snacks_M</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Vegetables_C</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Vegetables_H</t>
+        </is>
+      </c>
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Vegetables_L</t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t>Revenue_Vegetables_M</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Antigua and Barbuda </t>
+        </is>
+      </c>
+      <c r="B2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="6" t="n">
+        <v>2830544.64</v>
+      </c>
+      <c r="E2" s="6" t="n">
+        <v>978998.8</v>
+      </c>
+      <c r="F2" s="6" t="n">
+        <v>395068.7</v>
+      </c>
+      <c r="G2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="6" t="n">
+        <v>34069.1</v>
+      </c>
+      <c r="I2" s="6" t="n">
+        <v>96086.25</v>
+      </c>
+      <c r="J2" s="6" t="n">
+        <v>573903</v>
+      </c>
+      <c r="K2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" s="6" t="n">
+        <v>1246130.6</v>
+      </c>
+      <c r="M2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" s="6" t="n">
+        <v>197141.12</v>
+      </c>
+      <c r="Q2" s="6" t="n">
+        <v>2233136.8</v>
+      </c>
+      <c r="R2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" s="6" t="n">
+        <v>7516342.4</v>
+      </c>
+      <c r="V2" s="6" t="n">
+        <v>914.34</v>
+      </c>
+      <c r="W2" s="6" t="n">
+        <v>84520.47</v>
+      </c>
+      <c r="X2" s="6" t="n">
+        <v>163993.41</v>
+      </c>
+      <c r="Y2" s="6" t="n">
+        <v>7846.53</v>
+      </c>
+      <c r="Z2" s="6" t="n">
+        <v>8932765.09</v>
+      </c>
+      <c r="AA2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="6" t="n">
+        <v>668695.65</v>
+      </c>
+      <c r="AE2" s="6" t="n">
+        <v>1254278.97</v>
+      </c>
+      <c r="AF2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="6" t="n">
+        <v>10226601.84</v>
+      </c>
+      <c r="AI2" s="6" t="n">
+        <v>4634010.36</v>
+      </c>
+      <c r="AJ2" s="6" t="n">
+        <v>440217.96</v>
+      </c>
+      <c r="AK2" s="6" t="n">
+        <v>9876250.859999999</v>
+      </c>
+      <c r="AL2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM2" s="6" t="n">
+        <v>1520096.27</v>
+      </c>
+      <c r="AN2" s="6" t="n">
+        <v>1017538.5</v>
+      </c>
+      <c r="AO2" s="6" t="n">
+        <v>1520178</v>
+      </c>
+      <c r="AP2" s="6" t="n">
+        <v>46536.9</v>
+      </c>
+      <c r="AQ2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR2" s="6" t="n">
+        <v>1662359.1</v>
+      </c>
+      <c r="AS2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU2" s="6" t="n">
+        <v>69789.17999999999</v>
+      </c>
+      <c r="AV2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW2" s="6" t="n">
+        <v>616240</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Barbados</t>
+        </is>
+      </c>
+      <c r="B3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6" t="n">
+        <v>1385149.28</v>
+      </c>
+      <c r="E3" s="6" t="n">
+        <v>1210027.2</v>
+      </c>
+      <c r="F3" s="6" t="n">
+        <v>325222.3</v>
+      </c>
+      <c r="G3" s="6" t="n">
+        <v>102017.5</v>
+      </c>
+      <c r="H3" s="6" t="n">
+        <v>288021.5</v>
+      </c>
+      <c r="I3" s="6" t="n">
+        <v>472032.6</v>
+      </c>
+      <c r="J3" s="6" t="n">
+        <v>991268.3</v>
+      </c>
+      <c r="K3" s="6" t="n">
+        <v>1636960.6</v>
+      </c>
+      <c r="L3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" s="6" t="n">
+        <v>1496808.16</v>
+      </c>
+      <c r="O3" s="6" t="n">
+        <v>1825850.24</v>
+      </c>
+      <c r="P3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="6" t="n">
+        <v>677426.7200000001</v>
+      </c>
+      <c r="R3" s="6" t="n">
+        <v>11178766.8</v>
+      </c>
+      <c r="S3" s="6" t="n">
+        <v>1533697.6</v>
+      </c>
+      <c r="T3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" s="6" t="n">
+        <v>3915126</v>
+      </c>
+      <c r="V3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" s="6" t="n">
+        <v>295574.4</v>
+      </c>
+      <c r="X3" s="6" t="n">
+        <v>80853.78</v>
+      </c>
+      <c r="Y3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="6" t="n">
+        <v>4115874.93</v>
+      </c>
+      <c r="AA3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="6" t="n">
+        <v>1741561.92</v>
+      </c>
+      <c r="AE3" s="6" t="n">
+        <v>1801048.41</v>
+      </c>
+      <c r="AF3" s="6" t="n">
+        <v>2812318.74</v>
+      </c>
+      <c r="AG3" s="6" t="n">
+        <v>3735835.95</v>
+      </c>
+      <c r="AH3" s="6" t="n">
+        <v>7955832.57</v>
+      </c>
+      <c r="AI3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="6" t="n">
+        <v>2096244.99</v>
+      </c>
+      <c r="AL3" s="6" t="n">
+        <v>1291170.54</v>
+      </c>
+      <c r="AM3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP3" s="6" t="n">
+        <v>2054031.96</v>
+      </c>
+      <c r="AQ3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS3" s="6" t="n">
+        <v>1719576.6</v>
+      </c>
+      <c r="AT3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU3" s="6" t="n">
+        <v>775846.16</v>
+      </c>
+      <c r="AV3" s="6" t="n">
+        <v>670623.1800000001</v>
+      </c>
+      <c r="AW3" s="6" t="n">
+        <v>180250.2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Belize</t>
+        </is>
+      </c>
+      <c r="B4" s="6" t="n">
+        <v>2172177.52</v>
+      </c>
+      <c r="C4" s="6" t="n">
+        <v>3694922.72</v>
+      </c>
+      <c r="D4" s="6" t="n">
+        <v>2465749.52</v>
+      </c>
+      <c r="E4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6" t="n">
+        <v>754360.1</v>
+      </c>
+      <c r="G4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="6" t="n">
+        <v>777278.45</v>
+      </c>
+      <c r="I4" s="6" t="n">
+        <v>73784.75</v>
+      </c>
+      <c r="J4" s="6" t="n">
+        <v>757798.8</v>
+      </c>
+      <c r="K4" s="6" t="n">
+        <v>1937282.6</v>
+      </c>
+      <c r="L4" s="6" t="n">
+        <v>1108723</v>
+      </c>
+      <c r="M4" s="6" t="n">
+        <v>922770.2000000001</v>
+      </c>
+      <c r="N4" s="6" t="n">
+        <v>1277155.36</v>
+      </c>
+      <c r="O4" s="6" t="n">
+        <v>1428398.88</v>
+      </c>
+      <c r="P4" s="6" t="n">
+        <v>1501944.32</v>
+      </c>
+      <c r="Q4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" s="6" t="n">
+        <v>3125105.6</v>
+      </c>
+      <c r="S4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" s="6" t="n">
+        <v>5948543.2</v>
+      </c>
+      <c r="U4" s="6" t="n">
+        <v>8090823.199999999</v>
+      </c>
+      <c r="V4" s="6" t="n">
+        <v>72447.45</v>
+      </c>
+      <c r="W4" s="6" t="n">
+        <v>130302.78</v>
+      </c>
+      <c r="X4" s="6" t="n">
+        <v>27346.23</v>
+      </c>
+      <c r="Y4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="6" t="n">
+        <v>10211833.87</v>
+      </c>
+      <c r="AA4" s="6" t="n">
+        <v>11738830.82</v>
+      </c>
+      <c r="AB4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="6" t="n">
+        <v>3662119.6</v>
+      </c>
+      <c r="AD4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="6" t="n">
+        <v>2405616.78</v>
+      </c>
+      <c r="AF4" s="6" t="n">
+        <v>3791525.43</v>
+      </c>
+      <c r="AG4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="6" t="n">
+        <v>278717.88</v>
+      </c>
+      <c r="AI4" s="6" t="n">
+        <v>6215148.24</v>
+      </c>
+      <c r="AJ4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="6" t="n">
+        <v>2343053.58</v>
+      </c>
+      <c r="AL4" s="6" t="n">
+        <v>686205.08</v>
+      </c>
+      <c r="AM4" s="6" t="n">
+        <v>1225.95</v>
+      </c>
+      <c r="AN4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO4" s="6" t="n">
+        <v>683916.64</v>
+      </c>
+      <c r="AP4" s="6" t="n">
+        <v>1145112.9</v>
+      </c>
+      <c r="AQ4" s="6" t="n">
+        <v>2134289.04</v>
+      </c>
+      <c r="AR4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT4" s="6" t="n">
+        <v>3137740.02</v>
+      </c>
+      <c r="AU4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV4" s="6" t="n">
+        <v>2798345.84</v>
+      </c>
+      <c r="AW4" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Costa Rica</t>
+        </is>
+      </c>
+      <c r="B5" s="6" t="n">
+        <v>1634302.56</v>
+      </c>
+      <c r="C5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="6" t="n">
+        <v>905222.88</v>
+      </c>
+      <c r="E5" s="6" t="n">
+        <v>636923.6</v>
+      </c>
+      <c r="F5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="6" t="n">
+        <v>580218.6</v>
+      </c>
+      <c r="I5" s="6" t="n">
+        <v>359860.8</v>
+      </c>
+      <c r="J5" s="6" t="n">
+        <v>225447.2</v>
+      </c>
+      <c r="K5" s="6" t="n">
+        <v>1069434.3</v>
+      </c>
+      <c r="L5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" s="6" t="n">
+        <v>4078619.6</v>
+      </c>
+      <c r="N5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" s="6" t="n">
+        <v>1058813.92</v>
+      </c>
+      <c r="Q5" s="6" t="n">
+        <v>1658324</v>
+      </c>
+      <c r="R5" s="6" t="n">
+        <v>6039043.6</v>
+      </c>
+      <c r="S5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" s="6" t="n">
+        <v>3839490.4</v>
+      </c>
+      <c r="U5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="V5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X5" s="6" t="n">
+        <v>64918.14</v>
+      </c>
+      <c r="Y5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="6" t="n">
+        <v>74177.97</v>
+      </c>
+      <c r="AC5" s="6" t="n">
+        <v>1067895.46</v>
+      </c>
+      <c r="AD5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="6" t="n">
+        <v>2505182.82</v>
+      </c>
+      <c r="AF5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="6" t="n">
+        <v>2382412.83</v>
+      </c>
+      <c r="AH5" s="6" t="n">
+        <v>4738855.17</v>
+      </c>
+      <c r="AI5" s="6" t="n">
+        <v>5883031.14</v>
+      </c>
+      <c r="AJ5" s="6" t="n">
+        <v>2789783.64</v>
+      </c>
+      <c r="AK5" s="6" t="n">
+        <v>10563928.62</v>
+      </c>
+      <c r="AL5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM5" s="6" t="n">
+        <v>590826.17</v>
+      </c>
+      <c r="AN5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO5" s="6" t="n">
+        <v>965721.6799999999</v>
+      </c>
+      <c r="AP5" s="6" t="n">
+        <v>62862.96</v>
+      </c>
+      <c r="AQ5" s="6" t="n">
+        <v>858109.92</v>
+      </c>
+      <c r="AR5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS5" s="6" t="n">
+        <v>1521985.5</v>
+      </c>
+      <c r="AT5" s="6" t="n">
+        <v>1725626.06</v>
+      </c>
+      <c r="AU5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV5" s="6" t="n">
+        <v>915578.58</v>
+      </c>
+      <c r="AW5" s="6" t="n">
+        <v>4680804.98</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Cuba</t>
+        </is>
+      </c>
+      <c r="B6" s="6" t="n">
+        <v>1035160.4</v>
+      </c>
+      <c r="C6" s="6" t="n">
+        <v>3960158.64</v>
+      </c>
+      <c r="D6" s="6" t="n">
+        <v>1829591.76</v>
+      </c>
+      <c r="E6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="6" t="n">
+        <v>347381.45</v>
+      </c>
+      <c r="G6" s="6" t="n">
+        <v>94425.5</v>
+      </c>
+      <c r="H6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="6" t="n">
+        <v>2042601</v>
+      </c>
+      <c r="K6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="6" t="n">
+        <v>3247180.2</v>
+      </c>
+      <c r="M6" s="6" t="n">
+        <v>2013185.9</v>
+      </c>
+      <c r="N6" s="6" t="n">
+        <v>218122.88</v>
+      </c>
+      <c r="O6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" s="6" t="n">
+        <v>1397363.36</v>
+      </c>
+      <c r="Q6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" s="6" t="n">
+        <v>890576.4</v>
+      </c>
+      <c r="S6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" s="6" t="n">
+        <v>6864914.4</v>
+      </c>
+      <c r="U6" s="6" t="n">
+        <v>5489920.4</v>
+      </c>
+      <c r="V6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W6" s="6" t="n">
+        <v>253906.62</v>
+      </c>
+      <c r="X6" s="6" t="n">
+        <v>62240.43</v>
+      </c>
+      <c r="Y6" s="6" t="n">
+        <v>144195.15</v>
+      </c>
+      <c r="Z6" s="6" t="n">
+        <v>10075506.79</v>
+      </c>
+      <c r="AA6" s="6" t="n">
+        <v>970996.3100000001</v>
+      </c>
+      <c r="AB6" s="6" t="n">
+        <v>2647685.74</v>
+      </c>
+      <c r="AC6" s="6" t="n">
+        <v>4355783.86</v>
+      </c>
+      <c r="AD6" s="6" t="n">
+        <v>6874275.659999999</v>
+      </c>
+      <c r="AE6" s="6" t="n">
+        <v>620178.3</v>
+      </c>
+      <c r="AF6" s="6" t="n">
+        <v>1927615.41</v>
+      </c>
+      <c r="AG6" s="6" t="n">
+        <v>6049480.71</v>
+      </c>
+      <c r="AH6" s="6" t="n">
+        <v>5623849.56</v>
+      </c>
+      <c r="AI6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL6" s="6" t="n">
+        <v>627686.4</v>
+      </c>
+      <c r="AM6" s="6" t="n">
+        <v>1447928.68</v>
+      </c>
+      <c r="AN6" s="6" t="n">
+        <v>596792.46</v>
+      </c>
+      <c r="AO6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP6" s="6" t="n">
+        <v>648465</v>
+      </c>
+      <c r="AQ6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS6" s="6" t="n">
+        <v>826831.02</v>
+      </c>
+      <c r="AT6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV6" s="6" t="n">
+        <v>2787561.64</v>
+      </c>
+      <c r="AW6" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Dominica</t>
+        </is>
+      </c>
+      <c r="B7" s="6" t="n">
+        <v>1891624.8</v>
+      </c>
+      <c r="C7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="6" t="n">
+        <v>4466634.16</v>
+      </c>
+      <c r="E7" s="6" t="n">
+        <v>211371.84</v>
+      </c>
+      <c r="F7" s="6" t="n">
+        <v>820600.3</v>
+      </c>
+      <c r="G7" s="6" t="n">
+        <v>3701.1</v>
+      </c>
+      <c r="H7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="6" t="n">
+        <v>309658.7</v>
+      </c>
+      <c r="J7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" s="6" t="n">
+        <v>2043012.4</v>
+      </c>
+      <c r="N7" s="6" t="n">
+        <v>953577.28</v>
+      </c>
+      <c r="O7" s="6" t="n">
+        <v>1677338.72</v>
+      </c>
+      <c r="P7" s="6" t="n">
+        <v>963412.48</v>
+      </c>
+      <c r="Q7" s="6" t="n">
+        <v>296367.36</v>
+      </c>
+      <c r="R7" s="6" t="n">
+        <v>5806890.4</v>
+      </c>
+      <c r="S7" s="6" t="n">
+        <v>4211110.399999999</v>
+      </c>
+      <c r="T7" s="6" t="n">
+        <v>6852235.600000001</v>
+      </c>
+      <c r="U7" s="6" t="n">
+        <v>4094378</v>
+      </c>
+      <c r="V7" s="6" t="n">
+        <v>7454.67</v>
+      </c>
+      <c r="W7" s="6" t="n">
+        <v>29809.35</v>
+      </c>
+      <c r="X7" s="6" t="n">
+        <v>108367.95</v>
+      </c>
+      <c r="Y7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="6" t="n">
+        <v>3847230.39</v>
+      </c>
+      <c r="AA7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="6" t="n">
+        <v>8500394.4</v>
+      </c>
+      <c r="AC7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="6" t="n">
+        <v>2977699.62</v>
+      </c>
+      <c r="AE7" s="6" t="n">
+        <v>3601674.93</v>
+      </c>
+      <c r="AF7" s="6" t="n">
+        <v>720588.12</v>
+      </c>
+      <c r="AG7" s="6" t="n">
+        <v>3405074.19</v>
+      </c>
+      <c r="AH7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI7" s="6" t="n">
+        <v>11266584.21</v>
+      </c>
+      <c r="AJ7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL7" s="6" t="n">
+        <v>507379.84</v>
+      </c>
+      <c r="AM7" s="6" t="n">
+        <v>670022.5399999999</v>
+      </c>
+      <c r="AN7" s="6" t="n">
+        <v>897722.3200000001</v>
+      </c>
+      <c r="AO7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU7" s="6" t="n">
+        <v>2628263.6</v>
+      </c>
+      <c r="AV7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW7" s="6" t="n">
+        <v>1906030.32</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Dominican Republic</t>
+        </is>
+      </c>
+      <c r="B8" s="6" t="n">
+        <v>2786381.2</v>
+      </c>
+      <c r="C8" s="6" t="n">
+        <v>32675.84</v>
+      </c>
+      <c r="D8" s="6" t="n">
+        <v>4682601.039999999</v>
+      </c>
+      <c r="E8" s="6" t="n">
+        <v>300975.12</v>
+      </c>
+      <c r="F8" s="6" t="n">
+        <v>448592.3</v>
+      </c>
+      <c r="G8" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="6" t="n">
+        <v>1583684.3</v>
+      </c>
+      <c r="K8" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" s="6" t="n">
+        <v>12567.2</v>
+      </c>
+      <c r="O8" s="6" t="n">
+        <v>682672.1599999999</v>
+      </c>
+      <c r="P8" s="6" t="n">
+        <v>1309611.52</v>
+      </c>
+      <c r="Q8" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" s="6" t="n">
+        <v>3432020</v>
+      </c>
+      <c r="S8" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" s="6" t="n">
+        <v>4174385.6</v>
+      </c>
+      <c r="U8" s="6" t="n">
+        <v>3874466.4</v>
+      </c>
+      <c r="V8" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W8" s="6" t="n">
+        <v>91527.3</v>
+      </c>
+      <c r="X8" s="6" t="n">
+        <v>21505.65</v>
+      </c>
+      <c r="Y8" s="6" t="n">
+        <v>53358.27</v>
+      </c>
+      <c r="Z8" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="6" t="n">
+        <v>8948135.300000001</v>
+      </c>
+      <c r="AC8" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="6" t="n">
+        <v>3940452.6</v>
+      </c>
+      <c r="AE8" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="6" t="n">
+        <v>2783208.33</v>
+      </c>
+      <c r="AH8" s="6" t="n">
+        <v>1116825.15</v>
+      </c>
+      <c r="AI8" s="6" t="n">
+        <v>9574740.630000001</v>
+      </c>
+      <c r="AJ8" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK8" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL8" s="6" t="n">
+        <v>1307.68</v>
+      </c>
+      <c r="AM8" s="6" t="n">
+        <v>133955.47</v>
+      </c>
+      <c r="AN8" s="6" t="n">
+        <v>718651.89</v>
+      </c>
+      <c r="AO8" s="6" t="n">
+        <v>604229.8899999999</v>
+      </c>
+      <c r="AP8" s="6" t="n">
+        <v>183401.16</v>
+      </c>
+      <c r="AQ8" s="6" t="n">
+        <v>14037.36</v>
+      </c>
+      <c r="AR8" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS8" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT8" s="6" t="n">
+        <v>1490068.32</v>
+      </c>
+      <c r="AU8" s="6" t="n">
+        <v>544910.22</v>
+      </c>
+      <c r="AV8" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW8" s="6" t="n">
+        <v>859962.92</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>El Salvador</t>
+        </is>
+      </c>
+      <c r="B9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="6" t="n">
+        <v>2811653.92</v>
+      </c>
+      <c r="D9" s="6" t="n">
+        <v>3174917.36</v>
+      </c>
+      <c r="E9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="6" t="n">
+        <v>81519.10000000001</v>
+      </c>
+      <c r="G9" s="6" t="n">
+        <v>535473.25</v>
+      </c>
+      <c r="H9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="6" t="n">
+        <v>1363585.3</v>
+      </c>
+      <c r="K9" s="6" t="n">
+        <v>1935637</v>
+      </c>
+      <c r="L9" s="6" t="n">
+        <v>2644067.8</v>
+      </c>
+      <c r="M9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" s="6" t="n">
+        <v>827468.16</v>
+      </c>
+      <c r="O9" s="6" t="n">
+        <v>176815.04</v>
+      </c>
+      <c r="P9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" s="6" t="n">
+        <v>4957848</v>
+      </c>
+      <c r="S9" s="6" t="n">
+        <v>3057776.8</v>
+      </c>
+      <c r="T9" s="6" t="n">
+        <v>1395979.6</v>
+      </c>
+      <c r="U9" s="6" t="n">
+        <v>4557810</v>
+      </c>
+      <c r="V9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X9" s="6" t="n">
+        <v>110392.56</v>
+      </c>
+      <c r="Y9" s="6" t="n">
+        <v>109599.51</v>
+      </c>
+      <c r="Z9" s="6" t="n">
+        <v>10633512.24</v>
+      </c>
+      <c r="AA9" s="6" t="n">
+        <v>12985822.64</v>
+      </c>
+      <c r="AB9" s="6" t="n">
+        <v>7679758.84</v>
+      </c>
+      <c r="AC9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="6" t="n">
+        <v>8621322.15</v>
+      </c>
+      <c r="AE9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH9" s="6" t="n">
+        <v>8225433.51</v>
+      </c>
+      <c r="AI9" s="6" t="n">
+        <v>3236513.7</v>
+      </c>
+      <c r="AJ9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL9" s="6" t="n">
+        <v>543667.96</v>
+      </c>
+      <c r="AM9" s="6" t="n">
+        <v>127743.99</v>
+      </c>
+      <c r="AN9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO9" s="6" t="n">
+        <v>255733.17</v>
+      </c>
+      <c r="AP9" s="6" t="n">
+        <v>3180224.94</v>
+      </c>
+      <c r="AQ9" s="6" t="n">
+        <v>1225827.72</v>
+      </c>
+      <c r="AR9" s="6" t="n">
+        <v>2021074.68</v>
+      </c>
+      <c r="AS9" s="6" t="n">
+        <v>533114.52</v>
+      </c>
+      <c r="AT9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU9" s="6" t="n">
+        <v>938533.52</v>
+      </c>
+      <c r="AV9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW9" s="6" t="n">
+        <v>1323221.34</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Grenada</t>
+        </is>
+      </c>
+      <c r="B10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="6" t="n">
+        <v>2194642.16</v>
+      </c>
+      <c r="F10" s="6" t="n">
+        <v>164177</v>
+      </c>
+      <c r="G10" s="6" t="n">
+        <v>678250.3</v>
+      </c>
+      <c r="H10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="6" t="n">
+        <v>733624.45</v>
+      </c>
+      <c r="J10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="6" t="n">
+        <v>1955178.5</v>
+      </c>
+      <c r="M10" s="6" t="n">
+        <v>1439077.2</v>
+      </c>
+      <c r="N10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" s="6" t="n">
+        <v>427284.8</v>
+      </c>
+      <c r="Q10" s="6" t="n">
+        <v>556890.88</v>
+      </c>
+      <c r="R10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" s="6" t="n">
+        <v>13965042.4</v>
+      </c>
+      <c r="T10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="V10" s="6" t="n">
+        <v>28708.41</v>
+      </c>
+      <c r="W10" s="6" t="n">
+        <v>9647.219999999999</v>
+      </c>
+      <c r="X10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="6" t="n">
+        <v>4600370.68</v>
+      </c>
+      <c r="AB10" s="6" t="n">
+        <v>1645949.01</v>
+      </c>
+      <c r="AC10" s="6" t="n">
+        <v>3022585.21</v>
+      </c>
+      <c r="AD10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="6" t="n">
+        <v>7967392.65</v>
+      </c>
+      <c r="AF10" s="6" t="n">
+        <v>9403506.210000001</v>
+      </c>
+      <c r="AG10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH10" s="6" t="n">
+        <v>1204087.29</v>
+      </c>
+      <c r="AI10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ10" s="6" t="n">
+        <v>5575660.02</v>
+      </c>
+      <c r="AK10" s="6" t="n">
+        <v>2811273.57</v>
+      </c>
+      <c r="AL10" s="6" t="n">
+        <v>626869.1</v>
+      </c>
+      <c r="AM10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO10" s="6" t="n">
+        <v>759108.24</v>
+      </c>
+      <c r="AP10" s="6" t="n">
+        <v>1322868.6</v>
+      </c>
+      <c r="AQ10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR10" s="6" t="n">
+        <v>417306.3</v>
+      </c>
+      <c r="AS10" s="6" t="n">
+        <v>314467.38</v>
+      </c>
+      <c r="AT10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV10" s="6" t="n">
+        <v>2470506.16</v>
+      </c>
+      <c r="AW10" s="6" t="n">
+        <v>522263.4</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Guatemala</t>
+        </is>
+      </c>
+      <c r="B11" s="6" t="n">
+        <v>1046648</v>
+      </c>
+      <c r="C11" s="6" t="n">
+        <v>2500722.88</v>
+      </c>
+      <c r="D11" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="6" t="n">
+        <v>125884.85</v>
+      </c>
+      <c r="H11" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="6" t="n">
+        <v>770588</v>
+      </c>
+      <c r="J11" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" s="6" t="n">
+        <v>634378.8</v>
+      </c>
+      <c r="L11" s="6" t="n">
+        <v>2373983.7</v>
+      </c>
+      <c r="M11" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" s="6" t="n">
+        <v>314180</v>
+      </c>
+      <c r="O11" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P11" s="6" t="n">
+        <v>147965.12</v>
+      </c>
+      <c r="Q11" s="6" t="n">
+        <v>1701926.72</v>
+      </c>
+      <c r="R11" s="6" t="n">
+        <v>311286.4</v>
+      </c>
+      <c r="S11" s="6" t="n">
+        <v>5662614.4</v>
+      </c>
+      <c r="T11" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U11" s="6" t="n">
+        <v>8355329.199999999</v>
+      </c>
+      <c r="V11" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W11" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X11" s="6" t="n">
+        <v>50531.28</v>
+      </c>
+      <c r="Y11" s="6" t="n">
+        <v>61550.01</v>
+      </c>
+      <c r="Z11" s="6" t="n">
+        <v>4210101</v>
+      </c>
+      <c r="AA11" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="6" t="n">
+        <v>2250733.36</v>
+      </c>
+      <c r="AC11" s="6" t="n">
+        <v>5939583.76</v>
+      </c>
+      <c r="AD11" s="6" t="n">
+        <v>9065572.32</v>
+      </c>
+      <c r="AE11" s="6" t="n">
+        <v>3246443.55</v>
+      </c>
+      <c r="AF11" s="6" t="n">
+        <v>4119333.96</v>
+      </c>
+      <c r="AG11" s="6" t="n">
+        <v>4908690.15</v>
+      </c>
+      <c r="AH11" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI11" s="6" t="n">
+        <v>5614732.62</v>
+      </c>
+      <c r="AJ11" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK11" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL11" s="6" t="n">
+        <v>667488.91</v>
+      </c>
+      <c r="AM11" s="6" t="n">
+        <v>1265589.05</v>
+      </c>
+      <c r="AN11" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO11" s="6" t="n">
+        <v>500105.87</v>
+      </c>
+      <c r="AP11" s="6" t="n">
+        <v>301345.5</v>
+      </c>
+      <c r="AQ11" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR11" s="6" t="n">
+        <v>457129.68</v>
+      </c>
+      <c r="AS11" s="6" t="n">
+        <v>1286249.4</v>
+      </c>
+      <c r="AT11" s="6" t="n">
+        <v>470653.3</v>
+      </c>
+      <c r="AU11" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV11" s="6" t="n">
+        <v>1234020.6</v>
+      </c>
+      <c r="AW11" s="6" t="n">
+        <v>1702054.88</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Haiti</t>
+        </is>
+      </c>
+      <c r="B12" s="6" t="n">
+        <v>2635000.16</v>
+      </c>
+      <c r="C12" s="6" t="n">
+        <v>1702207.04</v>
+      </c>
+      <c r="D12" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="6" t="n">
+        <v>387004.48</v>
+      </c>
+      <c r="F12" s="6" t="n">
+        <v>38576.85</v>
+      </c>
+      <c r="G12" s="6" t="n">
+        <v>850066.75</v>
+      </c>
+      <c r="H12" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" s="6" t="n">
+        <v>1266906.3</v>
+      </c>
+      <c r="L12" s="6" t="n">
+        <v>1791647</v>
+      </c>
+      <c r="M12" s="6" t="n">
+        <v>1098643.7</v>
+      </c>
+      <c r="N12" s="6" t="n">
+        <v>2525132.96</v>
+      </c>
+      <c r="O12" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" s="6" t="n">
+        <v>475258.72</v>
+      </c>
+      <c r="Q12" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" s="6" t="n">
+        <v>450753.2</v>
+      </c>
+      <c r="S12" s="6" t="n">
+        <v>7264515.199999999</v>
+      </c>
+      <c r="T12" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U12" s="6" t="n">
+        <v>616452</v>
+      </c>
+      <c r="V12" s="6" t="n">
+        <v>75600.99000000001</v>
+      </c>
+      <c r="W12" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X12" s="6" t="n">
+        <v>15515.79</v>
+      </c>
+      <c r="Y12" s="6" t="n">
+        <v>122857.44</v>
+      </c>
+      <c r="Z12" s="6" t="n">
+        <v>1817694.4</v>
+      </c>
+      <c r="AA12" s="6" t="n">
+        <v>1273722.62</v>
+      </c>
+      <c r="AB12" s="6" t="n">
+        <v>10010684.6</v>
+      </c>
+      <c r="AC12" s="6" t="n">
+        <v>14647810.13</v>
+      </c>
+      <c r="AD12" s="6" t="n">
+        <v>3542188.44</v>
+      </c>
+      <c r="AE12" s="6" t="n">
+        <v>2604748.86</v>
+      </c>
+      <c r="AF12" s="6" t="n">
+        <v>2949854.88</v>
+      </c>
+      <c r="AG12" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH12" s="6" t="n">
+        <v>1788873.87</v>
+      </c>
+      <c r="AI12" s="6" t="n">
+        <v>6403347.93</v>
+      </c>
+      <c r="AJ12" s="6" t="n">
+        <v>1117476.36</v>
+      </c>
+      <c r="AK12" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL12" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM12" s="6" t="n">
+        <v>469702.31</v>
+      </c>
+      <c r="AN12" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO12" s="6" t="n">
+        <v>1922289.6</v>
+      </c>
+      <c r="AP12" s="6" t="n">
+        <v>1672276.8</v>
+      </c>
+      <c r="AQ12" s="6" t="n">
+        <v>1038306.9</v>
+      </c>
+      <c r="AR12" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS12" s="6" t="n">
+        <v>43027.56</v>
+      </c>
+      <c r="AT12" s="6" t="n">
+        <v>871209.3</v>
+      </c>
+      <c r="AU12" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV12" s="6" t="n">
+        <v>1381301.96</v>
+      </c>
+      <c r="AW12" s="6" t="n">
+        <v>3218005.28</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Honduras</t>
+        </is>
+      </c>
+      <c r="B13" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="6" t="n">
+        <v>2236252.8</v>
+      </c>
+      <c r="E13" s="6" t="n">
+        <v>235368.16</v>
+      </c>
+      <c r="F13" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="6" t="n">
+        <v>595782.2</v>
+      </c>
+      <c r="H13" s="6" t="n">
+        <v>811300.1</v>
+      </c>
+      <c r="I13" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" s="6" t="n">
+        <v>631704.7</v>
+      </c>
+      <c r="L13" s="6" t="n">
+        <v>3801130.3</v>
+      </c>
+      <c r="M13" s="6" t="n">
+        <v>417982.4</v>
+      </c>
+      <c r="N13" s="6" t="n">
+        <v>1085041.12</v>
+      </c>
+      <c r="O13" s="6" t="n">
+        <v>13004.32</v>
+      </c>
+      <c r="P13" s="6" t="n">
+        <v>1073566.72</v>
+      </c>
+      <c r="Q13" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" s="6" t="n">
+        <v>4312540.8</v>
+      </c>
+      <c r="T13" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U13" s="6" t="n">
+        <v>2684408</v>
+      </c>
+      <c r="V13" s="6" t="n">
+        <v>32440.41</v>
+      </c>
+      <c r="W13" s="6" t="n">
+        <v>19882.23</v>
+      </c>
+      <c r="X13" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="6" t="n">
+        <v>41807.73</v>
+      </c>
+      <c r="Z13" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="6" t="n">
+        <v>6206891.76</v>
+      </c>
+      <c r="AB13" s="6" t="n">
+        <v>5314083.04</v>
+      </c>
+      <c r="AC13" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE13" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF13" s="6" t="n">
+        <v>1656340.14</v>
+      </c>
+      <c r="AG13" s="6" t="n">
+        <v>899469.48</v>
+      </c>
+      <c r="AH13" s="6" t="n">
+        <v>2068242.96</v>
+      </c>
+      <c r="AI13" s="6" t="n">
+        <v>538550.67</v>
+      </c>
+      <c r="AJ13" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK13" s="6" t="n">
+        <v>1003514.61</v>
+      </c>
+      <c r="AL13" s="6" t="n">
+        <v>532634.41</v>
+      </c>
+      <c r="AM13" s="6" t="n">
+        <v>600715.5</v>
+      </c>
+      <c r="AN13" s="6" t="n">
+        <v>674435.96</v>
+      </c>
+      <c r="AO13" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP13" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ13" s="6" t="n">
+        <v>805469.8200000001</v>
+      </c>
+      <c r="AR13" s="6" t="n">
+        <v>1732240.74</v>
+      </c>
+      <c r="AS13" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT13" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU13" s="6" t="n">
+        <v>3128496.42</v>
+      </c>
+      <c r="AV13" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW13" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Jamaica</t>
+        </is>
+      </c>
+      <c r="B14" s="6" t="n">
+        <v>268809.84</v>
+      </c>
+      <c r="C14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="6" t="n">
+        <v>2198981.92</v>
+      </c>
+      <c r="E14" s="6" t="n">
+        <v>1706546.8</v>
+      </c>
+      <c r="F14" s="6" t="n">
+        <v>412530.3</v>
+      </c>
+      <c r="G14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="6" t="n">
+        <v>238531.15</v>
+      </c>
+      <c r="I14" s="6" t="n">
+        <v>316349.15</v>
+      </c>
+      <c r="J14" s="6" t="n">
+        <v>2204075.5</v>
+      </c>
+      <c r="K14" s="6" t="n">
+        <v>418188.1</v>
+      </c>
+      <c r="L14" s="6" t="n">
+        <v>1499964.4</v>
+      </c>
+      <c r="M14" s="6" t="n">
+        <v>1493999.1</v>
+      </c>
+      <c r="N14" s="6" t="n">
+        <v>185338.88</v>
+      </c>
+      <c r="O14" s="6" t="n">
+        <v>520063.52</v>
+      </c>
+      <c r="P14" s="6" t="n">
+        <v>675022.5600000001</v>
+      </c>
+      <c r="Q14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S14" s="6" t="n">
+        <v>6813324.800000001</v>
+      </c>
+      <c r="T14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="V14" s="6" t="n">
+        <v>69853.71000000001</v>
+      </c>
+      <c r="W14" s="6" t="n">
+        <v>23978.1</v>
+      </c>
+      <c r="X14" s="6" t="n">
+        <v>111960</v>
+      </c>
+      <c r="Y14" s="6" t="n">
+        <v>91536.63</v>
+      </c>
+      <c r="Z14" s="6" t="n">
+        <v>10910844.29</v>
+      </c>
+      <c r="AA14" s="6" t="n">
+        <v>5836670.18</v>
+      </c>
+      <c r="AB14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF14" s="6" t="n">
+        <v>3867043.74</v>
+      </c>
+      <c r="AG14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH14" s="6" t="n">
+        <v>1423545.06</v>
+      </c>
+      <c r="AI14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ14" s="6" t="n">
+        <v>8488522.350000001</v>
+      </c>
+      <c r="AK14" s="6" t="n">
+        <v>8881201.98</v>
+      </c>
+      <c r="AL14" s="6" t="n">
+        <v>592133.85</v>
+      </c>
+      <c r="AM14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN14" s="6" t="n">
+        <v>67182.06</v>
+      </c>
+      <c r="AO14" s="6" t="n">
+        <v>506317.35</v>
+      </c>
+      <c r="AP14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ14" s="6" t="n">
+        <v>827136.1800000001</v>
+      </c>
+      <c r="AR14" s="6" t="n">
+        <v>920820.3</v>
+      </c>
+      <c r="AS14" s="6" t="n">
+        <v>597655.86</v>
+      </c>
+      <c r="AT14" s="6" t="n">
+        <v>1167928.86</v>
+      </c>
+      <c r="AU14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW14" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Nicaragua</t>
+        </is>
+      </c>
+      <c r="B15" s="6" t="n">
+        <v>1739988.48</v>
+      </c>
+      <c r="C15" s="6" t="n">
+        <v>581017.28</v>
+      </c>
+      <c r="D15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="6" t="n">
+        <v>2723837.6</v>
+      </c>
+      <c r="F15" s="6" t="n">
+        <v>433503.2</v>
+      </c>
+      <c r="G15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" s="6" t="n">
+        <v>104390</v>
+      </c>
+      <c r="J15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" s="6" t="n">
+        <v>2407924.2</v>
+      </c>
+      <c r="L15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" s="6" t="n">
+        <v>541196.7</v>
+      </c>
+      <c r="N15" s="6" t="n">
+        <v>929972.8</v>
+      </c>
+      <c r="O15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P15" s="6" t="n">
+        <v>1016522.56</v>
+      </c>
+      <c r="Q15" s="6" t="n">
+        <v>130808.16</v>
+      </c>
+      <c r="R15" s="6" t="n">
+        <v>1568236.4</v>
+      </c>
+      <c r="S15" s="6" t="n">
+        <v>1191370</v>
+      </c>
+      <c r="T15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U15" s="6" t="n">
+        <v>2569861.6</v>
+      </c>
+      <c r="V15" s="6" t="n">
+        <v>70152.27</v>
+      </c>
+      <c r="W15" s="6" t="n">
+        <v>62940.18</v>
+      </c>
+      <c r="X15" s="6" t="n">
+        <v>23007.78</v>
+      </c>
+      <c r="Y15" s="6" t="n">
+        <v>13211.28</v>
+      </c>
+      <c r="Z15" s="6" t="n">
+        <v>7967114.939999999</v>
+      </c>
+      <c r="AA15" s="6" t="n">
+        <v>3378773.12</v>
+      </c>
+      <c r="AB15" s="6" t="n">
+        <v>10213170.41</v>
+      </c>
+      <c r="AC15" s="6" t="n">
+        <v>2434507.61</v>
+      </c>
+      <c r="AD15" s="6" t="n">
+        <v>3873793.98</v>
+      </c>
+      <c r="AE15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG15" s="6" t="n">
+        <v>2770973.52</v>
+      </c>
+      <c r="AH15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI15" s="6" t="n">
+        <v>7634786.04</v>
+      </c>
+      <c r="AJ15" s="6" t="n">
+        <v>2458968.96</v>
+      </c>
+      <c r="AK15" s="6" t="n">
+        <v>3904003.95</v>
+      </c>
+      <c r="AL15" s="6" t="n">
+        <v>687839.6800000001</v>
+      </c>
+      <c r="AM15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN15" s="6" t="n">
+        <v>116056.6</v>
+      </c>
+      <c r="AO15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP15" s="6" t="n">
+        <v>1448899.68</v>
+      </c>
+      <c r="AQ15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS15" s="6" t="n">
+        <v>41044.02</v>
+      </c>
+      <c r="AT15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU15" s="6" t="n">
+        <v>403483.14</v>
+      </c>
+      <c r="AV15" s="6" t="n">
+        <v>1988144.3</v>
+      </c>
+      <c r="AW15" s="6" t="n">
+        <v>1401946</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Panama</t>
+        </is>
+      </c>
+      <c r="B16" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" s="6" t="n">
+        <v>2024880.96</v>
+      </c>
+      <c r="D16" s="6" t="n">
+        <v>3120798</v>
+      </c>
+      <c r="E16" s="6" t="n">
+        <v>3701049.44</v>
+      </c>
+      <c r="F16" s="6" t="n">
+        <v>76679.2</v>
+      </c>
+      <c r="G16" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="6" t="n">
+        <v>508664</v>
+      </c>
+      <c r="I16" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" s="6" t="n">
+        <v>307110.1</v>
+      </c>
+      <c r="K16" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" s="6" t="n">
+        <v>2112539</v>
+      </c>
+      <c r="N16" s="6" t="n">
+        <v>1179021.92</v>
+      </c>
+      <c r="O16" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P16" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R16" s="6" t="n">
+        <v>5396359.6</v>
+      </c>
+      <c r="S16" s="6" t="n">
+        <v>1971334.8</v>
+      </c>
+      <c r="T16" s="6" t="n">
+        <v>6359074</v>
+      </c>
+      <c r="U16" s="6" t="n">
+        <v>1600589.2</v>
+      </c>
+      <c r="V16" s="6" t="n">
+        <v>53143.68</v>
+      </c>
+      <c r="W16" s="6" t="n">
+        <v>25060.38</v>
+      </c>
+      <c r="X16" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="6" t="n">
+        <v>24388.62</v>
+      </c>
+      <c r="Z16" s="6" t="n">
+        <v>192461.76</v>
+      </c>
+      <c r="AA16" s="6" t="n">
+        <v>6978075.34</v>
+      </c>
+      <c r="AB16" s="6" t="n">
+        <v>4232153.91</v>
+      </c>
+      <c r="AC16" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD16" s="6" t="n">
+        <v>1793032.5</v>
+      </c>
+      <c r="AE16" s="6" t="n">
+        <v>1798095.18</v>
+      </c>
+      <c r="AF16" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG16" s="6" t="n">
+        <v>6554904.93</v>
+      </c>
+      <c r="AH16" s="6" t="n">
+        <v>3686499.81</v>
+      </c>
+      <c r="AI16" s="6" t="n">
+        <v>272856.99</v>
+      </c>
+      <c r="AJ16" s="6" t="n">
+        <v>1280278.86</v>
+      </c>
+      <c r="AK16" s="6" t="n">
+        <v>72935.52</v>
+      </c>
+      <c r="AL16" s="6" t="n">
+        <v>284665.59</v>
+      </c>
+      <c r="AM16" s="6" t="n">
+        <v>679748.4099999999</v>
+      </c>
+      <c r="AN16" s="6" t="n">
+        <v>857184.24</v>
+      </c>
+      <c r="AO16" s="6" t="n">
+        <v>839530.5600000001</v>
+      </c>
+      <c r="AP16" s="6" t="n">
+        <v>1806547.2</v>
+      </c>
+      <c r="AQ16" s="6" t="n">
+        <v>1669988.1</v>
+      </c>
+      <c r="AR16" s="6" t="n">
+        <v>3680229.6</v>
+      </c>
+      <c r="AS16" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT16" s="6" t="n">
+        <v>1987990.24</v>
+      </c>
+      <c r="AU16" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV16" s="6" t="n">
+        <v>2250816.6</v>
+      </c>
+      <c r="AW16" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Saint Kitts and Nevis </t>
+        </is>
+      </c>
+      <c r="B17" s="6" t="n">
+        <v>1341496.4</v>
+      </c>
+      <c r="C17" s="6" t="n">
+        <v>1751731.36</v>
+      </c>
+      <c r="D17" s="6" t="n">
+        <v>2598495.12</v>
+      </c>
+      <c r="E17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" s="6" t="n">
+        <v>3938.35</v>
+      </c>
+      <c r="J17" s="6" t="n">
+        <v>1584095.7</v>
+      </c>
+      <c r="K17" s="6" t="n">
+        <v>2417180.7</v>
+      </c>
+      <c r="L17" s="6" t="n">
+        <v>706990.9</v>
+      </c>
+      <c r="M17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" s="6" t="n">
+        <v>759386.72</v>
+      </c>
+      <c r="O17" s="6" t="n">
+        <v>807251.36</v>
+      </c>
+      <c r="P17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R17" s="6" t="n">
+        <v>496222</v>
+      </c>
+      <c r="S17" s="6" t="n">
+        <v>1389421.6</v>
+      </c>
+      <c r="T17" s="6" t="n">
+        <v>3896326.4</v>
+      </c>
+      <c r="U17" s="6" t="n">
+        <v>2621014</v>
+      </c>
+      <c r="V17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W17" s="6" t="n">
+        <v>125460.51</v>
+      </c>
+      <c r="X17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="6" t="n">
+        <v>14340.21</v>
+      </c>
+      <c r="Z17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="6" t="n">
+        <v>651563.25</v>
+      </c>
+      <c r="AB17" s="6" t="n">
+        <v>2080992.78</v>
+      </c>
+      <c r="AC17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH17" s="6" t="n">
+        <v>834851.22</v>
+      </c>
+      <c r="AI17" s="6" t="n">
+        <v>12079945.5</v>
+      </c>
+      <c r="AJ17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK17" s="6" t="n">
+        <v>6736767.45</v>
+      </c>
+      <c r="AL17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM17" s="6" t="n">
+        <v>195007.78</v>
+      </c>
+      <c r="AN17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO17" s="6" t="n">
+        <v>1360395.85</v>
+      </c>
+      <c r="AP17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ17" s="6" t="n">
+        <v>212696.52</v>
+      </c>
+      <c r="AR17" s="6" t="n">
+        <v>5173377.48</v>
+      </c>
+      <c r="AS17" s="6" t="n">
+        <v>317366.4</v>
+      </c>
+      <c r="AT17" s="6" t="n">
+        <v>59467.16</v>
+      </c>
+      <c r="AU17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV17" s="6" t="n">
+        <v>2037751.62</v>
+      </c>
+      <c r="AW17" s="6" t="n">
+        <v>1781087.66</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Saint Lucia</t>
+        </is>
+      </c>
+      <c r="B18" s="6" t="n">
+        <v>719634.3199999999</v>
+      </c>
+      <c r="C18" s="6" t="n">
+        <v>2013138.08</v>
+      </c>
+      <c r="D18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="6" t="n">
+        <v>704572.8</v>
+      </c>
+      <c r="F18" s="6" t="n">
+        <v>742307.8</v>
+      </c>
+      <c r="G18" s="6" t="n">
+        <v>212433.65</v>
+      </c>
+      <c r="H18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" s="6" t="n">
+        <v>162516.25</v>
+      </c>
+      <c r="J18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" s="6" t="n">
+        <v>1857471</v>
+      </c>
+      <c r="L18" s="6" t="n">
+        <v>281191.9</v>
+      </c>
+      <c r="M18" s="6" t="n">
+        <v>163325.8</v>
+      </c>
+      <c r="N18" s="6" t="n">
+        <v>892599.04</v>
+      </c>
+      <c r="O18" s="6" t="n">
+        <v>695676.48</v>
+      </c>
+      <c r="P18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="6" t="n">
+        <v>327.84</v>
+      </c>
+      <c r="R18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S18" s="6" t="n">
+        <v>4885710</v>
+      </c>
+      <c r="T18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="V18" s="6" t="n">
+        <v>89521.35000000001</v>
+      </c>
+      <c r="W18" s="6" t="n">
+        <v>78773.19</v>
+      </c>
+      <c r="X18" s="6" t="n">
+        <v>70413.50999999999</v>
+      </c>
+      <c r="Y18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="6" t="n">
+        <v>3422878.94</v>
+      </c>
+      <c r="AC18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="6" t="n">
+        <v>2962089.69</v>
+      </c>
+      <c r="AF18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG18" s="6" t="n">
+        <v>1762234.53</v>
+      </c>
+      <c r="AH18" s="6" t="n">
+        <v>11192346.27</v>
+      </c>
+      <c r="AI18" s="6" t="n">
+        <v>5561333.4</v>
+      </c>
+      <c r="AJ18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK18" s="6" t="n">
+        <v>10614071.79</v>
+      </c>
+      <c r="AL18" s="6" t="n">
+        <v>1188272.47</v>
+      </c>
+      <c r="AM18" s="6" t="n">
+        <v>805367.42</v>
+      </c>
+      <c r="AN18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO18" s="6" t="n">
+        <v>102080.77</v>
+      </c>
+      <c r="AP18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR18" s="6" t="n">
+        <v>272660.46</v>
+      </c>
+      <c r="AS18" s="6" t="n">
+        <v>3101646.24</v>
+      </c>
+      <c r="AT18" s="6" t="n">
+        <v>2070720.46</v>
+      </c>
+      <c r="AU18" s="6" t="n">
+        <v>693424.0600000001</v>
+      </c>
+      <c r="AV18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW18" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Saint Vincent and the Grenadines</t>
+        </is>
+      </c>
+      <c r="B19" s="6" t="n">
+        <v>1357579.04</v>
+      </c>
+      <c r="C19" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="6" t="n">
+        <v>3956074.16</v>
+      </c>
+      <c r="F19" s="6" t="n">
+        <v>790564.45</v>
+      </c>
+      <c r="G19" s="6" t="n">
+        <v>460407.35</v>
+      </c>
+      <c r="H19" s="6" t="n">
+        <v>371106.45</v>
+      </c>
+      <c r="I19" s="6" t="n">
+        <v>180642.15</v>
+      </c>
+      <c r="J19" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" s="6" t="n">
+        <v>1811394.2</v>
+      </c>
+      <c r="L19" s="6" t="n">
+        <v>1000113.4</v>
+      </c>
+      <c r="M19" s="6" t="n">
+        <v>1319771.2</v>
+      </c>
+      <c r="N19" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O19" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P19" s="6" t="n">
+        <v>1377037.28</v>
+      </c>
+      <c r="Q19" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R19" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S19" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T19" s="6" t="n">
+        <v>4115800.8</v>
+      </c>
+      <c r="U19" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="V19" s="6" t="n">
+        <v>150950.07</v>
+      </c>
+      <c r="W19" s="6" t="n">
+        <v>71262.53999999999</v>
+      </c>
+      <c r="X19" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="6" t="n">
+        <v>3920071.82</v>
+      </c>
+      <c r="AA19" s="6" t="n">
+        <v>1218256.21</v>
+      </c>
+      <c r="AB19" s="6" t="n">
+        <v>2054930.25</v>
+      </c>
+      <c r="AC19" s="6" t="n">
+        <v>1597165.3</v>
+      </c>
+      <c r="AD19" s="6" t="n">
+        <v>3727398.15</v>
+      </c>
+      <c r="AE19" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF19" s="6" t="n">
+        <v>3192019.74</v>
+      </c>
+      <c r="AG19" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH19" s="6" t="n">
+        <v>8551689.719999999</v>
+      </c>
+      <c r="AI19" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ19" s="6" t="n">
+        <v>3543233.61</v>
+      </c>
+      <c r="AK19" s="6" t="n">
+        <v>11261374.53</v>
+      </c>
+      <c r="AL19" s="6" t="n">
+        <v>537374.75</v>
+      </c>
+      <c r="AM19" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN19" s="6" t="n">
+        <v>1650700.81</v>
+      </c>
+      <c r="AO19" s="6" t="n">
+        <v>975529.2799999999</v>
+      </c>
+      <c r="AP19" s="6" t="n">
+        <v>1090031.52</v>
+      </c>
+      <c r="AQ19" s="6" t="n">
+        <v>1702029.9</v>
+      </c>
+      <c r="AR19" s="6" t="n">
+        <v>1369558.08</v>
+      </c>
+      <c r="AS19" s="6" t="n">
+        <v>198964.32</v>
+      </c>
+      <c r="AT19" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU19" s="6" t="n">
+        <v>1674632.2</v>
+      </c>
+      <c r="AV19" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW19" s="6" t="n">
+        <v>934682.02</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>The Bahamas</t>
+        </is>
+      </c>
+      <c r="B20" s="6" t="n">
+        <v>4458465.2</v>
+      </c>
+      <c r="C20" s="6" t="n">
+        <v>969808.72</v>
+      </c>
+      <c r="D20" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="6" t="n">
+        <v>145007.2</v>
+      </c>
+      <c r="G20" s="6" t="n">
+        <v>352079</v>
+      </c>
+      <c r="H20" s="6" t="n">
+        <v>513930.95</v>
+      </c>
+      <c r="I20" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" s="6" t="n">
+        <v>1480011.5</v>
+      </c>
+      <c r="K20" s="6" t="n">
+        <v>4216438.6</v>
+      </c>
+      <c r="L20" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" s="6" t="n">
+        <v>483189.3</v>
+      </c>
+      <c r="N20" s="6" t="n">
+        <v>3232939.52</v>
+      </c>
+      <c r="O20" s="6" t="n">
+        <v>449577.92</v>
+      </c>
+      <c r="P20" s="6" t="n">
+        <v>2359355.2</v>
+      </c>
+      <c r="Q20" s="6" t="n">
+        <v>1951959.36</v>
+      </c>
+      <c r="R20" s="6" t="n">
+        <v>1024359.6</v>
+      </c>
+      <c r="S20" s="6" t="n">
+        <v>1623323.6</v>
+      </c>
+      <c r="T20" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U20" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="V20" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W20" s="6" t="n">
+        <v>63938.49000000001</v>
+      </c>
+      <c r="X20" s="6" t="n">
+        <v>29240.22</v>
+      </c>
+      <c r="Y20" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="6" t="n">
+        <v>3680162.89</v>
+      </c>
+      <c r="AB20" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="6" t="n">
+        <v>6267704.33</v>
+      </c>
+      <c r="AD20" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE20" s="6" t="n">
+        <v>2096793.3</v>
+      </c>
+      <c r="AF20" s="6" t="n">
+        <v>1865175.69</v>
+      </c>
+      <c r="AG20" s="6" t="n">
+        <v>1476193.11</v>
+      </c>
+      <c r="AH20" s="6" t="n">
+        <v>2086476.84</v>
+      </c>
+      <c r="AI20" s="6" t="n">
+        <v>4585169.61</v>
+      </c>
+      <c r="AJ20" s="6" t="n">
+        <v>4843699.98</v>
+      </c>
+      <c r="AK20" s="6" t="n">
+        <v>6381206.79</v>
+      </c>
+      <c r="AL20" s="6" t="n">
+        <v>155368.73</v>
+      </c>
+      <c r="AM20" s="6" t="n">
+        <v>1258642</v>
+      </c>
+      <c r="AN20" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO20" s="6" t="n">
+        <v>1009774.15</v>
+      </c>
+      <c r="AP20" s="6" t="n">
+        <v>296310.36</v>
+      </c>
+      <c r="AQ20" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR20" s="6" t="n">
+        <v>389841.9</v>
+      </c>
+      <c r="AS20" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT20" s="6" t="n">
+        <v>190880.34</v>
+      </c>
+      <c r="AU20" s="6" t="n">
+        <v>1045759.28</v>
+      </c>
+      <c r="AV20" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW20" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Trinidad and Tobago</t>
+        </is>
+      </c>
+      <c r="B21" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" s="6" t="n">
+        <v>141935.68</v>
+      </c>
+      <c r="D21" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" s="6" t="n">
+        <v>22159.15</v>
+      </c>
+      <c r="J21" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" s="6" t="n">
+        <v>1334581.6</v>
+      </c>
+      <c r="L21" s="6" t="n">
+        <v>2997049</v>
+      </c>
+      <c r="M21" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N21" s="6" t="n">
+        <v>322594.56</v>
+      </c>
+      <c r="O21" s="6" t="n">
+        <v>1356711.2</v>
+      </c>
+      <c r="P21" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="6" t="n">
+        <v>434278.72</v>
+      </c>
+      <c r="R21" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S21" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T21" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U21" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="V21" s="6" t="n">
+        <v>129714.99</v>
+      </c>
+      <c r="W21" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X21" s="6" t="n">
+        <v>90239.75999999999</v>
+      </c>
+      <c r="Y21" s="6" t="n">
+        <v>32841.6</v>
+      </c>
+      <c r="Z21" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA21" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="6" t="n">
+        <v>6055862.74</v>
+      </c>
+      <c r="AC21" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD21" s="6" t="n">
+        <v>1898083.11</v>
+      </c>
+      <c r="AE21" s="6" t="n">
+        <v>1036583.73</v>
+      </c>
+      <c r="AF21" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG21" s="6" t="n">
+        <v>7898624.58</v>
+      </c>
+      <c r="AH21" s="6" t="n">
+        <v>4790951.97</v>
+      </c>
+      <c r="AI21" s="6" t="n">
+        <v>2038287.3</v>
+      </c>
+      <c r="AJ21" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK21" s="6" t="n">
+        <v>2783271.54</v>
+      </c>
+      <c r="AL21" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM21" s="6" t="n">
+        <v>126926.69</v>
+      </c>
+      <c r="AN21" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO21" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP21" s="6" t="n">
+        <v>1850337.66</v>
+      </c>
+      <c r="AQ21" s="6" t="n">
+        <v>858415.08</v>
+      </c>
+      <c r="AR21" s="6" t="n">
+        <v>2614305.72</v>
+      </c>
+      <c r="AS21" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT21" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU21" s="6" t="n">
+        <v>381144.44</v>
+      </c>
+      <c r="AV21" s="6" t="n">
+        <v>399323.52</v>
+      </c>
+      <c r="AW21" s="6" t="n">
+        <v>1900021.98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added a second seaborn plot
</commit_message>
<xml_diff>
--- a/data/Sales Records processed.xlsx
+++ b/data/Sales Records processed.xlsx
@@ -199,6 +199,31 @@
       </nvPicPr>
       <blipFill>
         <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>1</col>
+      <colOff>0</colOff>
+      <row>79</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="19050000" cy="14287500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>

</xml_diff>

<commit_message>
added a second pie chart
</commit_message>
<xml_diff>
--- a/data/Sales Records processed.xlsx
+++ b/data/Sales Records processed.xlsx
@@ -224,6 +224,31 @@
       </nvPicPr>
       <blipFill>
         <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>1</col>
+      <colOff>0</colOff>
+      <row>159</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="19050000" cy="14287500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId3"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>

</xml_diff>